<commit_message>
Fix loi tim kiem San Pham va chinh sua giao dien
</commit_message>
<xml_diff>
--- a/test-case.xlsx
+++ b/test-case.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kiemthutest\newupdate_thu7\CuaHangDoChoi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="-150" windowWidth="12120" windowHeight="9060" tabRatio="821" activeTab="1"/>
+    <workbookView xWindow="1635" yWindow="300" windowWidth="12120" windowHeight="9060" tabRatio="821" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -24,7 +29,7 @@
     <definedName name="Port">[1]Validation!$F$2:$F$40</definedName>
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1357,7 +1362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -2442,26 +2447,6 @@
     <xf numFmtId="14" fontId="25" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="24" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2483,12 +2468,138 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="24" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2498,228 +2609,122 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="24" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="24" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2732,6 +2737,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -5074,7 +5082,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5109,7 +5117,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5392,11 +5400,11 @@
       <c r="B6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="157"/>
-      <c r="E6" s="158"/>
+      <c r="D6" s="170"/>
+      <c r="E6" s="171"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
@@ -5405,11 +5413,11 @@
       <c r="B7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="157" t="s">
+      <c r="C7" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="157"/>
-      <c r="E7" s="158"/>
+      <c r="D7" s="170"/>
+      <c r="E7" s="171"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
@@ -5622,8 +5630,8 @@
   </sheetPr>
   <dimension ref="A1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -5642,9 +5650,9 @@
       <c r="A1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
+      <c r="B1" s="197"/>
+      <c r="C1" s="197"/>
+      <c r="D1" s="197"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -5655,9 +5663,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="181"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5670,51 +5678,51 @@
       <c r="A3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="157" t="s">
+      <c r="B3" s="170" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="171"/>
       <c r="E3" s="68"/>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="187"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="188" t="s">
+      <c r="B4" s="206" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="189"/>
-      <c r="D4" s="190"/>
+      <c r="C4" s="207"/>
+      <c r="D4" s="208"/>
       <c r="E4" s="68"/>
       <c r="F4" s="68"/>
       <c r="G4" s="68"/>
-      <c r="H4" s="187"/>
-      <c r="I4" s="187"/>
-      <c r="J4" s="187"/>
+      <c r="H4" s="204"/>
+      <c r="I4" s="204"/>
+      <c r="J4" s="204"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="81" customFormat="1" ht="12.75">
       <c r="A5" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="200" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="185"/>
+      <c r="C5" s="201"/>
+      <c r="D5" s="202"/>
       <c r="E5" s="79"/>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
-      <c r="H5" s="186"/>
-      <c r="I5" s="186"/>
-      <c r="J5" s="186"/>
+      <c r="H5" s="203"/>
+      <c r="I5" s="203"/>
+      <c r="J5" s="203"/>
       <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -5723,7 +5731,7 @@
       </c>
       <c r="B6" s="95">
         <f>COUNTIF(I12:I138,"Pass")</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>70</v>
@@ -5735,9 +5743,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
+      <c r="H6" s="204"/>
+      <c r="I6" s="204"/>
+      <c r="J6" s="204"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -5746,7 +5754,7 @@
       </c>
       <c r="B7" s="96">
         <f>COUNTIF(I12:I138,"Fail")</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>71</v>
@@ -5758,16 +5766,16 @@
       <c r="E7" s="69"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
-      <c r="H7" s="187"/>
-      <c r="I7" s="187"/>
-      <c r="J7" s="187"/>
+      <c r="H7" s="204"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="204"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="182"/>
-      <c r="B8" s="182"/>
-      <c r="C8" s="182"/>
-      <c r="D8" s="182"/>
+      <c r="A8" s="199"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="199"/>
+      <c r="D8" s="199"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -5777,86 +5785,86 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="83" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="167" t="s">
+      <c r="A9" s="213" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="214" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="167" t="s">
+      <c r="C9" s="213" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="216" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="191" t="s">
+      <c r="E9" s="217"/>
+      <c r="F9" s="217"/>
+      <c r="G9" s="218"/>
+      <c r="H9" s="209" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="168" t="s">
+      <c r="I9" s="205" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="168" t="s">
+      <c r="J9" s="205" t="s">
         <v>79</v>
       </c>
       <c r="K9" s="82"/>
     </row>
     <row r="10" spans="1:11" s="71" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="168"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="172"/>
-      <c r="E10" s="173"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="192"/>
-      <c r="I10" s="168"/>
-      <c r="J10" s="168"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="205"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="221"/>
+      <c r="H10" s="210"/>
+      <c r="I10" s="205"/>
+      <c r="J10" s="205"/>
       <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:11" s="84" customFormat="1" ht="15">
-      <c r="A11" s="193"/>
-      <c r="B11" s="193"/>
-      <c r="C11" s="193"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="193"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="194"/>
+      <c r="A11" s="211"/>
+      <c r="B11" s="211"/>
+      <c r="C11" s="211"/>
+      <c r="D11" s="211"/>
+      <c r="E11" s="211"/>
+      <c r="F11" s="211"/>
+      <c r="G11" s="211"/>
+      <c r="H11" s="211"/>
+      <c r="I11" s="211"/>
+      <c r="J11" s="212"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="159" t="s">
+      <c r="A12" s="193" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="160"/>
-      <c r="C12" s="160"/>
-      <c r="D12" s="160"/>
-      <c r="E12" s="160"/>
-      <c r="F12" s="160"/>
-      <c r="G12" s="160"/>
-      <c r="H12" s="160"/>
-      <c r="I12" s="160"/>
-      <c r="J12" s="161"/>
+      <c r="B12" s="194"/>
+      <c r="C12" s="194"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="194"/>
+      <c r="G12" s="194"/>
+      <c r="H12" s="194"/>
+      <c r="I12" s="194"/>
+      <c r="J12" s="195"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="162" t="s">
+      <c r="D13" s="178" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
+      <c r="E13" s="179"/>
+      <c r="F13" s="179"/>
       <c r="G13" s="86"/>
       <c r="H13" s="122">
         <v>43774</v>
@@ -5870,17 +5878,17 @@
       <c r="A14" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="216" t="s">
+      <c r="B14" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="162" t="s">
+      <c r="D14" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="179"/>
       <c r="G14" s="86"/>
       <c r="H14" s="122">
         <v>43774</v>
@@ -5894,17 +5902,17 @@
       <c r="A15" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="216" t="s">
+      <c r="B15" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="162" t="s">
+      <c r="D15" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="163"/>
-      <c r="F15" s="163"/>
+      <c r="E15" s="179"/>
+      <c r="F15" s="179"/>
       <c r="G15" s="86"/>
       <c r="H15" s="122">
         <v>43774</v>
@@ -5918,17 +5926,17 @@
       <c r="A16" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="216" t="s">
+      <c r="B16" s="156" t="s">
         <v>86</v>
       </c>
       <c r="C16" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="162" t="s">
+      <c r="D16" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="179"/>
       <c r="G16" s="86"/>
       <c r="H16" s="122">
         <v>43774</v>
@@ -5942,17 +5950,17 @@
       <c r="A17" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="216" t="s">
+      <c r="B17" s="156" t="s">
         <v>86</v>
       </c>
       <c r="C17" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="162" t="s">
+      <c r="D17" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
+      <c r="E17" s="179"/>
+      <c r="F17" s="179"/>
       <c r="G17" s="86"/>
       <c r="H17" s="122">
         <v>43774</v>
@@ -5966,17 +5974,17 @@
       <c r="A18" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="216" t="s">
+      <c r="B18" s="156" t="s">
         <v>86</v>
       </c>
       <c r="C18" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="162" t="s">
+      <c r="D18" s="178" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="163"/>
-      <c r="F18" s="163"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
       <c r="G18" s="86"/>
       <c r="H18" s="122">
         <v>43774</v>
@@ -5990,17 +5998,17 @@
       <c r="A19" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="216" t="s">
+      <c r="B19" s="156" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="162" t="s">
+      <c r="D19" s="178" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="163"/>
-      <c r="F19" s="163"/>
+      <c r="E19" s="179"/>
+      <c r="F19" s="179"/>
       <c r="G19" s="86"/>
       <c r="H19" s="122">
         <v>43774</v>
@@ -6014,17 +6022,17 @@
       <c r="A20" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="216" t="s">
+      <c r="B20" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C20" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="162" t="s">
+      <c r="D20" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="163"/>
-      <c r="F20" s="163"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="179"/>
       <c r="G20" s="86"/>
       <c r="H20" s="122">
         <v>43774</v>
@@ -6038,17 +6046,17 @@
       <c r="A21" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="216" t="s">
+      <c r="B21" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C21" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="162" t="s">
+      <c r="D21" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="163"/>
-      <c r="F21" s="163"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="179"/>
       <c r="G21" s="86"/>
       <c r="H21" s="122">
         <v>43774</v>
@@ -6062,17 +6070,17 @@
       <c r="A22" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="216" t="s">
+      <c r="B22" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C22" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="162" t="s">
+      <c r="D22" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="163"/>
-      <c r="F22" s="163"/>
+      <c r="E22" s="179"/>
+      <c r="F22" s="179"/>
       <c r="G22" s="86"/>
       <c r="H22" s="122">
         <v>43774</v>
@@ -6086,17 +6094,17 @@
       <c r="A23" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="216" t="s">
+      <c r="B23" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C23" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="162" t="s">
+      <c r="D23" s="178" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="163"/>
-      <c r="F23" s="163"/>
+      <c r="E23" s="179"/>
+      <c r="F23" s="179"/>
       <c r="G23" s="86"/>
       <c r="H23" s="122">
         <v>43774</v>
@@ -6107,23 +6115,23 @@
       <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" ht="21.75" customHeight="1" outlineLevel="1">
-      <c r="A24" s="177"/>
-      <c r="B24" s="178"/>
-      <c r="C24" s="178"/>
-      <c r="D24" s="178"/>
-      <c r="E24" s="178"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="178"/>
-      <c r="H24" s="178"/>
-      <c r="I24" s="178"/>
-      <c r="J24" s="179"/>
+      <c r="A24" s="222"/>
+      <c r="B24" s="223"/>
+      <c r="C24" s="223"/>
+      <c r="D24" s="223"/>
+      <c r="E24" s="223"/>
+      <c r="F24" s="223"/>
+      <c r="G24" s="223"/>
+      <c r="H24" s="223"/>
+      <c r="I24" s="223"/>
+      <c r="J24" s="224"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="159" t="s">
+      <c r="A25" s="193" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="160"/>
-      <c r="C25" s="160"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="194"/>
       <c r="D25" s="113"/>
       <c r="E25" s="113"/>
       <c r="F25" s="113"/>
@@ -6133,812 +6141,812 @@
       <c r="J25" s="114"/>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A26" s="196" t="s">
+      <c r="A26" s="185" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="197"/>
-      <c r="C26" s="197"/>
-      <c r="D26" s="197"/>
-      <c r="E26" s="197"/>
-      <c r="F26" s="197"/>
-      <c r="G26" s="197"/>
-      <c r="H26" s="197"/>
-      <c r="I26" s="197"/>
-      <c r="J26" s="198"/>
-    </row>
-    <row r="27" spans="1:10" s="212" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
-      <c r="A27" s="206" t="s">
+      <c r="B26" s="186"/>
+      <c r="C26" s="186"/>
+      <c r="D26" s="186"/>
+      <c r="E26" s="186"/>
+      <c r="F26" s="186"/>
+      <c r="G26" s="186"/>
+      <c r="H26" s="186"/>
+      <c r="I26" s="186"/>
+      <c r="J26" s="187"/>
+    </row>
+    <row r="27" spans="1:10" s="154" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+      <c r="A27" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="207" t="s">
+      <c r="B27" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="208" t="s">
+      <c r="C27" s="151" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="213" t="s">
+      <c r="D27" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="209"/>
-      <c r="F27" s="209"/>
-      <c r="G27" s="210"/>
-      <c r="H27" s="214">
+      <c r="E27" s="176"/>
+      <c r="F27" s="176"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="155">
         <v>43774</v>
       </c>
       <c r="I27" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J27" s="211"/>
-    </row>
-    <row r="28" spans="1:10" s="212" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
-      <c r="A28" s="206" t="s">
+      <c r="J27" s="153"/>
+    </row>
+    <row r="28" spans="1:10" s="154" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
+      <c r="A28" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="207" t="s">
+      <c r="B28" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="208" t="s">
+      <c r="C28" s="151" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="213" t="s">
+      <c r="D28" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="209"/>
-      <c r="F28" s="209"/>
-      <c r="G28" s="210"/>
-      <c r="H28" s="214">
+      <c r="E28" s="176"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="155">
         <v>43774</v>
       </c>
       <c r="I28" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J28" s="211"/>
-    </row>
-    <row r="29" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A29" s="206" t="s">
+      <c r="J28" s="153"/>
+    </row>
+    <row r="29" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A29" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="207" t="s">
+      <c r="B29" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="208" t="s">
+      <c r="C29" s="151" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="213" t="s">
+      <c r="D29" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="209"/>
-      <c r="F29" s="209"/>
-      <c r="G29" s="210"/>
-      <c r="H29" s="214">
+      <c r="E29" s="176"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="155">
         <v>43774</v>
       </c>
       <c r="I29" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J29" s="211"/>
-    </row>
-    <row r="30" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A30" s="206" t="s">
+      <c r="J29" s="153"/>
+    </row>
+    <row r="30" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A30" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="207" t="s">
+      <c r="B30" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="208" t="s">
+      <c r="C30" s="151" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="213" t="s">
+      <c r="D30" s="175" t="s">
         <v>135</v>
       </c>
-      <c r="E30" s="209"/>
-      <c r="F30" s="209"/>
-      <c r="G30" s="210"/>
-      <c r="H30" s="214">
+      <c r="E30" s="176"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="155">
         <v>43774</v>
       </c>
       <c r="I30" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J30" s="211"/>
-    </row>
-    <row r="31" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A31" s="206" t="s">
+      <c r="J30" s="153"/>
+    </row>
+    <row r="31" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A31" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="207" t="s">
+      <c r="B31" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="208" t="s">
+      <c r="C31" s="151" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="213" t="s">
+      <c r="D31" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E31" s="209"/>
-      <c r="F31" s="209"/>
-      <c r="G31" s="210"/>
-      <c r="H31" s="214">
+      <c r="E31" s="176"/>
+      <c r="F31" s="176"/>
+      <c r="G31" s="152"/>
+      <c r="H31" s="155">
         <v>43774</v>
       </c>
       <c r="I31" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J31" s="211"/>
-    </row>
-    <row r="32" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A32" s="206" t="s">
+      <c r="J31" s="153"/>
+    </row>
+    <row r="32" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A32" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="207" t="s">
+      <c r="B32" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="208" t="s">
+      <c r="C32" s="151" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="213" t="s">
+      <c r="D32" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="209"/>
-      <c r="F32" s="209"/>
-      <c r="G32" s="210"/>
-      <c r="H32" s="214">
+      <c r="E32" s="176"/>
+      <c r="F32" s="176"/>
+      <c r="G32" s="152"/>
+      <c r="H32" s="155">
         <v>43774</v>
       </c>
       <c r="I32" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="211"/>
-    </row>
-    <row r="33" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A33" s="206" t="s">
+      <c r="J32" s="153"/>
+    </row>
+    <row r="33" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A33" s="149" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="207" t="s">
+      <c r="B33" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="208" t="s">
+      <c r="C33" s="151" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="213" t="s">
+      <c r="D33" s="175" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="209"/>
-      <c r="F33" s="209"/>
-      <c r="G33" s="210"/>
-      <c r="H33" s="214">
+      <c r="E33" s="176"/>
+      <c r="F33" s="176"/>
+      <c r="G33" s="152"/>
+      <c r="H33" s="155">
         <v>43774</v>
       </c>
       <c r="I33" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J33" s="211"/>
-    </row>
-    <row r="34" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A34" s="206" t="s">
+      <c r="J33" s="153"/>
+    </row>
+    <row r="34" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A34" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="207" t="s">
+      <c r="B34" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="208" t="s">
+      <c r="C34" s="151" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="213" t="s">
+      <c r="D34" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="209"/>
-      <c r="F34" s="209"/>
-      <c r="G34" s="210"/>
-      <c r="H34" s="214">
+      <c r="E34" s="176"/>
+      <c r="F34" s="176"/>
+      <c r="G34" s="152"/>
+      <c r="H34" s="155">
         <v>43774</v>
       </c>
       <c r="I34" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J34" s="211"/>
-    </row>
-    <row r="35" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A35" s="206" t="s">
+      <c r="J34" s="153"/>
+    </row>
+    <row r="35" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A35" s="149" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="207" t="s">
+      <c r="B35" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="208" t="s">
+      <c r="C35" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="D35" s="213" t="s">
+      <c r="D35" s="175" t="s">
         <v>138</v>
       </c>
-      <c r="E35" s="209"/>
-      <c r="F35" s="209"/>
-      <c r="G35" s="210"/>
-      <c r="H35" s="214">
+      <c r="E35" s="176"/>
+      <c r="F35" s="176"/>
+      <c r="G35" s="152"/>
+      <c r="H35" s="155">
         <v>43774</v>
       </c>
       <c r="I35" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J35" s="211"/>
-    </row>
-    <row r="36" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A36" s="206" t="s">
+      <c r="J35" s="153"/>
+    </row>
+    <row r="36" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A36" s="149" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="207" t="s">
+      <c r="B36" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="208" t="s">
+      <c r="C36" s="151" t="s">
         <v>139</v>
       </c>
-      <c r="D36" s="213" t="s">
+      <c r="D36" s="175" t="s">
         <v>138</v>
       </c>
-      <c r="E36" s="209"/>
-      <c r="F36" s="209"/>
-      <c r="G36" s="210"/>
-      <c r="H36" s="214">
+      <c r="E36" s="176"/>
+      <c r="F36" s="176"/>
+      <c r="G36" s="152"/>
+      <c r="H36" s="155">
         <v>43774</v>
       </c>
       <c r="I36" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="211"/>
-    </row>
-    <row r="37" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A37" s="206" t="s">
+      <c r="J36" s="153"/>
+    </row>
+    <row r="37" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A37" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="207" t="s">
+      <c r="B37" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="208" t="s">
+      <c r="C37" s="151" t="s">
         <v>141</v>
       </c>
-      <c r="D37" s="213" t="s">
+      <c r="D37" s="175" t="s">
         <v>140</v>
       </c>
-      <c r="E37" s="209"/>
-      <c r="F37" s="209"/>
-      <c r="G37" s="210"/>
-      <c r="H37" s="214">
+      <c r="E37" s="176"/>
+      <c r="F37" s="176"/>
+      <c r="G37" s="152"/>
+      <c r="H37" s="155">
         <v>43774</v>
       </c>
       <c r="I37" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J37" s="211"/>
-    </row>
-    <row r="38" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A38" s="206" t="s">
+      <c r="J37" s="153"/>
+    </row>
+    <row r="38" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A38" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="207" t="s">
+      <c r="B38" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C38" s="208" t="s">
+      <c r="C38" s="151" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="213" t="s">
+      <c r="D38" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E38" s="209"/>
-      <c r="F38" s="209"/>
-      <c r="G38" s="210"/>
-      <c r="H38" s="214">
+      <c r="E38" s="176"/>
+      <c r="F38" s="176"/>
+      <c r="G38" s="152"/>
+      <c r="H38" s="155">
         <v>43774</v>
       </c>
       <c r="I38" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J38" s="211"/>
-    </row>
-    <row r="39" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A39" s="206" t="s">
+      <c r="J38" s="153"/>
+    </row>
+    <row r="39" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A39" s="149" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="207" t="s">
+      <c r="B39" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="208" t="s">
+      <c r="C39" s="151" t="s">
         <v>144</v>
       </c>
-      <c r="D39" s="213" t="s">
+      <c r="D39" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="209"/>
-      <c r="F39" s="209"/>
-      <c r="G39" s="210"/>
-      <c r="H39" s="214">
+      <c r="E39" s="176"/>
+      <c r="F39" s="176"/>
+      <c r="G39" s="152"/>
+      <c r="H39" s="155">
         <v>43774</v>
       </c>
       <c r="I39" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="211"/>
-    </row>
-    <row r="40" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A40" s="206" t="s">
+      <c r="J39" s="153"/>
+    </row>
+    <row r="40" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A40" s="149" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="207" t="s">
+      <c r="B40" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="208" t="s">
+      <c r="C40" s="151" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="213" t="s">
+      <c r="D40" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="209"/>
-      <c r="F40" s="209"/>
-      <c r="G40" s="210"/>
-      <c r="H40" s="214">
+      <c r="E40" s="176"/>
+      <c r="F40" s="176"/>
+      <c r="G40" s="152"/>
+      <c r="H40" s="155">
         <v>43774</v>
       </c>
       <c r="I40" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J40" s="211"/>
-    </row>
-    <row r="41" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A41" s="206" t="s">
+      <c r="J40" s="153"/>
+    </row>
+    <row r="41" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A41" s="149" t="s">
         <v>146</v>
       </c>
-      <c r="B41" s="207" t="s">
+      <c r="B41" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="208" t="s">
+      <c r="C41" s="151" t="s">
         <v>147</v>
       </c>
-      <c r="D41" s="213" t="s">
+      <c r="D41" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="209"/>
-      <c r="F41" s="209"/>
-      <c r="G41" s="210"/>
-      <c r="H41" s="214">
+      <c r="E41" s="176"/>
+      <c r="F41" s="176"/>
+      <c r="G41" s="152"/>
+      <c r="H41" s="155">
         <v>43774</v>
       </c>
       <c r="I41" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J41" s="211"/>
-    </row>
-    <row r="42" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A42" s="206" t="s">
+      <c r="J41" s="153"/>
+    </row>
+    <row r="42" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A42" s="149" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="207" t="s">
+      <c r="B42" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="208" t="s">
+      <c r="C42" s="151" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="213" t="s">
+      <c r="D42" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="209"/>
-      <c r="F42" s="209"/>
-      <c r="G42" s="210"/>
-      <c r="H42" s="214">
+      <c r="E42" s="176"/>
+      <c r="F42" s="176"/>
+      <c r="G42" s="152"/>
+      <c r="H42" s="155">
         <v>43774</v>
       </c>
       <c r="I42" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J42" s="211"/>
-    </row>
-    <row r="43" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A43" s="206" t="s">
+      <c r="J42" s="153"/>
+    </row>
+    <row r="43" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A43" s="149" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="207" t="s">
+      <c r="B43" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="208" t="s">
+      <c r="C43" s="151" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="213" t="s">
+      <c r="D43" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="E43" s="209"/>
-      <c r="F43" s="209"/>
-      <c r="G43" s="210"/>
-      <c r="H43" s="214">
+      <c r="E43" s="176"/>
+      <c r="F43" s="176"/>
+      <c r="G43" s="152"/>
+      <c r="H43" s="155">
         <v>43774</v>
       </c>
       <c r="I43" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J43" s="211"/>
-    </row>
-    <row r="44" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A44" s="206" t="s">
+      <c r="J43" s="153"/>
+    </row>
+    <row r="44" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A44" s="149" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="207" t="s">
+      <c r="B44" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="208" t="s">
+      <c r="C44" s="151" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="213" t="s">
+      <c r="D44" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="E44" s="209"/>
-      <c r="F44" s="209"/>
-      <c r="G44" s="210"/>
-      <c r="H44" s="214">
+      <c r="E44" s="176"/>
+      <c r="F44" s="176"/>
+      <c r="G44" s="152"/>
+      <c r="H44" s="155">
         <v>43774</v>
       </c>
       <c r="I44" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J44" s="211"/>
-    </row>
-    <row r="45" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A45" s="206" t="s">
+      <c r="J44" s="153"/>
+    </row>
+    <row r="45" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A45" s="149" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="207" t="s">
+      <c r="B45" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="208" t="s">
+      <c r="C45" s="151" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="213" t="s">
+      <c r="D45" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E45" s="209"/>
-      <c r="F45" s="209"/>
-      <c r="G45" s="210"/>
-      <c r="H45" s="214">
+      <c r="E45" s="176"/>
+      <c r="F45" s="176"/>
+      <c r="G45" s="152"/>
+      <c r="H45" s="155">
         <v>43774</v>
       </c>
       <c r="I45" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J45" s="211"/>
-    </row>
-    <row r="46" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A46" s="206" t="s">
+      <c r="J45" s="153"/>
+    </row>
+    <row r="46" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A46" s="149" t="s">
         <v>158</v>
       </c>
-      <c r="B46" s="207" t="s">
+      <c r="B46" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="208" t="s">
+      <c r="C46" s="151" t="s">
         <v>159</v>
       </c>
-      <c r="D46" s="213" t="s">
+      <c r="D46" s="175" t="s">
         <v>153</v>
       </c>
-      <c r="E46" s="209"/>
-      <c r="F46" s="209"/>
-      <c r="G46" s="210"/>
-      <c r="H46" s="214">
+      <c r="E46" s="176"/>
+      <c r="F46" s="176"/>
+      <c r="G46" s="152"/>
+      <c r="H46" s="155">
         <v>43774</v>
       </c>
       <c r="I46" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J46" s="211"/>
-    </row>
-    <row r="47" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A47" s="206" t="s">
+      <c r="J46" s="153"/>
+    </row>
+    <row r="47" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A47" s="149" t="s">
         <v>160</v>
       </c>
-      <c r="B47" s="207" t="s">
+      <c r="B47" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="208" t="s">
+      <c r="C47" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="D47" s="213" t="s">
+      <c r="D47" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="209"/>
-      <c r="F47" s="209"/>
-      <c r="G47" s="210"/>
-      <c r="H47" s="214">
+      <c r="E47" s="176"/>
+      <c r="F47" s="176"/>
+      <c r="G47" s="152"/>
+      <c r="H47" s="155">
         <v>43774</v>
       </c>
       <c r="I47" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J47" s="211"/>
-    </row>
-    <row r="48" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A48" s="206" t="s">
+      <c r="J47" s="153"/>
+    </row>
+    <row r="48" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A48" s="149" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="207" t="s">
+      <c r="B48" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="208" t="s">
+      <c r="C48" s="151" t="s">
         <v>163</v>
       </c>
-      <c r="D48" s="213" t="s">
+      <c r="D48" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E48" s="209"/>
-      <c r="F48" s="209"/>
-      <c r="G48" s="210"/>
-      <c r="H48" s="214">
+      <c r="E48" s="176"/>
+      <c r="F48" s="176"/>
+      <c r="G48" s="152"/>
+      <c r="H48" s="155">
         <v>43774</v>
       </c>
       <c r="I48" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J48" s="211"/>
-    </row>
-    <row r="49" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A49" s="206" t="s">
+      <c r="J48" s="153"/>
+    </row>
+    <row r="49" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A49" s="149" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="207" t="s">
+      <c r="B49" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="208" t="s">
+      <c r="C49" s="151" t="s">
         <v>165</v>
       </c>
-      <c r="D49" s="213" t="s">
+      <c r="D49" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="209"/>
-      <c r="F49" s="209"/>
-      <c r="G49" s="210"/>
-      <c r="H49" s="214">
+      <c r="E49" s="176"/>
+      <c r="F49" s="176"/>
+      <c r="G49" s="152"/>
+      <c r="H49" s="155">
         <v>43774</v>
       </c>
       <c r="I49" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J49" s="211"/>
-    </row>
-    <row r="50" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A50" s="206" t="s">
+      <c r="J49" s="153"/>
+    </row>
+    <row r="50" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A50" s="149" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="207" t="s">
+      <c r="B50" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="208" t="s">
+      <c r="C50" s="151" t="s">
         <v>167</v>
       </c>
-      <c r="D50" s="213" t="s">
+      <c r="D50" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="209"/>
-      <c r="F50" s="209"/>
-      <c r="G50" s="210"/>
-      <c r="H50" s="214">
+      <c r="E50" s="176"/>
+      <c r="F50" s="176"/>
+      <c r="G50" s="152"/>
+      <c r="H50" s="155">
         <v>43774</v>
       </c>
       <c r="I50" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J50" s="211"/>
-    </row>
-    <row r="51" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A51" s="206" t="s">
+      <c r="J50" s="153"/>
+    </row>
+    <row r="51" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A51" s="149" t="s">
         <v>168</v>
       </c>
-      <c r="B51" s="207" t="s">
+      <c r="B51" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="208" t="s">
+      <c r="C51" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D51" s="213" t="s">
+      <c r="D51" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="209"/>
-      <c r="F51" s="209"/>
-      <c r="G51" s="210"/>
-      <c r="H51" s="214">
+      <c r="E51" s="176"/>
+      <c r="F51" s="176"/>
+      <c r="G51" s="152"/>
+      <c r="H51" s="155">
         <v>43774</v>
       </c>
       <c r="I51" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J51" s="211"/>
-    </row>
-    <row r="52" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A52" s="206" t="s">
+      <c r="J51" s="153"/>
+    </row>
+    <row r="52" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A52" s="149" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="207" t="s">
+      <c r="B52" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="208" t="s">
+      <c r="C52" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="213" t="s">
+      <c r="D52" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E52" s="209"/>
-      <c r="F52" s="209"/>
-      <c r="G52" s="210"/>
-      <c r="H52" s="214">
+      <c r="E52" s="176"/>
+      <c r="F52" s="176"/>
+      <c r="G52" s="152"/>
+      <c r="H52" s="155">
         <v>43774</v>
       </c>
       <c r="I52" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J52" s="211"/>
-    </row>
-    <row r="53" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A53" s="206" t="s">
+      <c r="J52" s="153"/>
+    </row>
+    <row r="53" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A53" s="149" t="s">
         <v>172</v>
       </c>
-      <c r="B53" s="207" t="s">
+      <c r="B53" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="208" t="s">
+      <c r="C53" s="151" t="s">
         <v>173</v>
       </c>
-      <c r="D53" s="213" t="s">
+      <c r="D53" s="175" t="s">
         <v>174</v>
       </c>
-      <c r="E53" s="209"/>
-      <c r="F53" s="209"/>
-      <c r="G53" s="210"/>
-      <c r="H53" s="214">
+      <c r="E53" s="176"/>
+      <c r="F53" s="176"/>
+      <c r="G53" s="152"/>
+      <c r="H53" s="155">
         <v>43774</v>
       </c>
       <c r="I53" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J53" s="211"/>
-    </row>
-    <row r="54" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A54" s="206" t="s">
+      <c r="J53" s="153"/>
+    </row>
+    <row r="54" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A54" s="149" t="s">
         <v>175</v>
       </c>
-      <c r="B54" s="207" t="s">
+      <c r="B54" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="208" t="s">
+      <c r="C54" s="151" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="213" t="s">
+      <c r="D54" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="209"/>
-      <c r="F54" s="209"/>
-      <c r="G54" s="210"/>
-      <c r="H54" s="214">
+      <c r="E54" s="176"/>
+      <c r="F54" s="176"/>
+      <c r="G54" s="152"/>
+      <c r="H54" s="155">
         <v>43774</v>
       </c>
       <c r="I54" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J54" s="211"/>
-    </row>
-    <row r="55" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A55" s="206" t="s">
+      <c r="J54" s="153"/>
+    </row>
+    <row r="55" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A55" s="149" t="s">
         <v>177</v>
       </c>
-      <c r="B55" s="207" t="s">
+      <c r="B55" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="208" t="s">
+      <c r="C55" s="151" t="s">
         <v>178</v>
       </c>
-      <c r="D55" s="213" t="s">
+      <c r="D55" s="175" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="209"/>
-      <c r="F55" s="209"/>
-      <c r="G55" s="210"/>
-      <c r="H55" s="214">
+      <c r="E55" s="176"/>
+      <c r="F55" s="176"/>
+      <c r="G55" s="152"/>
+      <c r="H55" s="155">
         <v>43774</v>
       </c>
       <c r="I55" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J55" s="211"/>
-    </row>
-    <row r="56" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A56" s="206" t="s">
+      <c r="J55" s="153"/>
+    </row>
+    <row r="56" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A56" s="149" t="s">
         <v>180</v>
       </c>
-      <c r="B56" s="207" t="s">
+      <c r="B56" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="208" t="s">
+      <c r="C56" s="151" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="213" t="s">
+      <c r="D56" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E56" s="209"/>
-      <c r="F56" s="209"/>
-      <c r="G56" s="210"/>
-      <c r="H56" s="214">
+      <c r="E56" s="176"/>
+      <c r="F56" s="176"/>
+      <c r="G56" s="152"/>
+      <c r="H56" s="155">
         <v>43774</v>
       </c>
       <c r="I56" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J56" s="211"/>
-    </row>
-    <row r="57" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A57" s="206" t="s">
+      <c r="J56" s="153"/>
+    </row>
+    <row r="57" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A57" s="149" t="s">
         <v>181</v>
       </c>
-      <c r="B57" s="207" t="s">
+      <c r="B57" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="208" t="s">
+      <c r="C57" s="151" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="213" t="s">
+      <c r="D57" s="175" t="s">
         <v>127</v>
       </c>
-      <c r="E57" s="209"/>
-      <c r="F57" s="209"/>
-      <c r="G57" s="210"/>
-      <c r="H57" s="214">
+      <c r="E57" s="176"/>
+      <c r="F57" s="176"/>
+      <c r="G57" s="152"/>
+      <c r="H57" s="155">
         <v>43774</v>
       </c>
       <c r="I57" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J57" s="211"/>
-    </row>
-    <row r="58" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A58" s="206" t="s">
+      <c r="J57" s="153"/>
+    </row>
+    <row r="58" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A58" s="149" t="s">
         <v>182</v>
       </c>
-      <c r="B58" s="207" t="s">
+      <c r="B58" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="208" t="s">
+      <c r="C58" s="151" t="s">
         <v>190</v>
       </c>
-      <c r="D58" s="213" t="s">
+      <c r="D58" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E58" s="209"/>
-      <c r="F58" s="209"/>
-      <c r="G58" s="210"/>
-      <c r="H58" s="214">
+      <c r="E58" s="176"/>
+      <c r="F58" s="176"/>
+      <c r="G58" s="152"/>
+      <c r="H58" s="155">
         <v>43774</v>
       </c>
       <c r="I58" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J58" s="211"/>
-    </row>
-    <row r="59" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A59" s="206" t="s">
+      <c r="J58" s="153"/>
+    </row>
+    <row r="59" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A59" s="149" t="s">
         <v>183</v>
       </c>
-      <c r="B59" s="207" t="s">
+      <c r="B59" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="208" t="s">
+      <c r="C59" s="151" t="s">
         <v>191</v>
       </c>
-      <c r="D59" s="213" t="s">
+      <c r="D59" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E59" s="209"/>
-      <c r="F59" s="209"/>
-      <c r="G59" s="210"/>
-      <c r="H59" s="214">
+      <c r="E59" s="176"/>
+      <c r="F59" s="176"/>
+      <c r="G59" s="152"/>
+      <c r="H59" s="155">
         <v>43774</v>
       </c>
       <c r="I59" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J59" s="211"/>
-    </row>
-    <row r="60" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="J59" s="153"/>
+    </row>
+    <row r="60" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
       <c r="A60" s="115" t="s">
         <v>184</v>
       </c>
@@ -6948,11 +6956,11 @@
       <c r="C60" s="117" t="s">
         <v>192</v>
       </c>
-      <c r="D60" s="215" t="s">
+      <c r="D60" s="172" t="s">
         <v>128</v>
       </c>
-      <c r="E60" s="176"/>
-      <c r="F60" s="176"/>
+      <c r="E60" s="173"/>
+      <c r="F60" s="173"/>
       <c r="G60" s="118"/>
       <c r="H60" s="121">
         <v>43774</v>
@@ -6964,79 +6972,79 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A61" s="206" t="s">
+    <row r="61" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A61" s="149" t="s">
         <v>185</v>
       </c>
-      <c r="B61" s="207" t="s">
+      <c r="B61" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C61" s="208" t="s">
+      <c r="C61" s="151" t="s">
         <v>194</v>
       </c>
-      <c r="D61" s="213" t="s">
+      <c r="D61" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E61" s="209"/>
-      <c r="F61" s="209"/>
-      <c r="G61" s="210"/>
-      <c r="H61" s="214">
+      <c r="E61" s="176"/>
+      <c r="F61" s="176"/>
+      <c r="G61" s="152"/>
+      <c r="H61" s="155">
         <v>43774</v>
       </c>
       <c r="I61" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J61" s="211"/>
-    </row>
-    <row r="62" spans="1:10" s="212" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
-      <c r="A62" s="206" t="s">
+      <c r="J61" s="153"/>
+    </row>
+    <row r="62" spans="1:10" s="154" customFormat="1" ht="99" customHeight="1" outlineLevel="1">
+      <c r="A62" s="149" t="s">
         <v>186</v>
       </c>
-      <c r="B62" s="207" t="s">
+      <c r="B62" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C62" s="208" t="s">
+      <c r="C62" s="151" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="213" t="s">
+      <c r="D62" s="175" t="s">
         <v>128</v>
       </c>
-      <c r="E62" s="209"/>
-      <c r="F62" s="209"/>
-      <c r="G62" s="210"/>
-      <c r="H62" s="214">
+      <c r="E62" s="176"/>
+      <c r="F62" s="176"/>
+      <c r="G62" s="152"/>
+      <c r="H62" s="155">
         <v>43774</v>
       </c>
       <c r="I62" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J62" s="211"/>
-    </row>
-    <row r="63" spans="1:10" s="212" customFormat="1" ht="106.5" customHeight="1" outlineLevel="1">
-      <c r="A63" s="206" t="s">
+      <c r="J62" s="153"/>
+    </row>
+    <row r="63" spans="1:10" s="154" customFormat="1" ht="106.5" customHeight="1" outlineLevel="1">
+      <c r="A63" s="149" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="207" t="s">
+      <c r="B63" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C63" s="208" t="s">
+      <c r="C63" s="151" t="s">
         <v>196</v>
       </c>
-      <c r="D63" s="213" t="s">
+      <c r="D63" s="175" t="s">
         <v>197</v>
       </c>
-      <c r="E63" s="209"/>
-      <c r="F63" s="209"/>
-      <c r="G63" s="210"/>
-      <c r="H63" s="214">
+      <c r="E63" s="176"/>
+      <c r="F63" s="176"/>
+      <c r="G63" s="152"/>
+      <c r="H63" s="155">
         <v>43774</v>
       </c>
       <c r="I63" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J63" s="211"/>
-    </row>
-    <row r="64" spans="1:10" s="212" customFormat="1" ht="106.5" customHeight="1" outlineLevel="1">
+      <c r="J63" s="153"/>
+    </row>
+    <row r="64" spans="1:10" s="154" customFormat="1" ht="106.5" customHeight="1" outlineLevel="1">
       <c r="A64" s="115" t="s">
         <v>198</v>
       </c>
@@ -7046,13 +7054,13 @@
       <c r="C64" s="117" t="s">
         <v>199</v>
       </c>
-      <c r="D64" s="215" t="s">
+      <c r="D64" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="E64" s="176"/>
-      <c r="F64" s="176"/>
+      <c r="E64" s="173"/>
+      <c r="F64" s="173"/>
       <c r="G64" s="118"/>
-      <c r="H64" s="217">
+      <c r="H64" s="157">
         <v>43774</v>
       </c>
       <c r="I64" s="119" t="s">
@@ -7062,104 +7070,104 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="222" customFormat="1" ht="106.5" customHeight="1" outlineLevel="1">
-      <c r="A65" s="223" t="s">
+    <row r="65" spans="1:10" s="162" customFormat="1" ht="106.5" customHeight="1" outlineLevel="1">
+      <c r="A65" s="163" t="s">
         <v>202</v>
       </c>
-      <c r="B65" s="207" t="s">
+      <c r="B65" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C65" s="208" t="s">
+      <c r="C65" s="151" t="s">
         <v>203</v>
       </c>
-      <c r="D65" s="227" t="s">
+      <c r="D65" s="181" t="s">
         <v>127</v>
       </c>
-      <c r="E65" s="228"/>
-      <c r="F65" s="228"/>
-      <c r="G65" s="224"/>
-      <c r="H65" s="214">
+      <c r="E65" s="182"/>
+      <c r="F65" s="182"/>
+      <c r="G65" s="164"/>
+      <c r="H65" s="155">
         <v>43774</v>
       </c>
-      <c r="I65" s="225" t="s">
+      <c r="I65" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="J65" s="226"/>
-    </row>
-    <row r="66" spans="1:10" s="222" customFormat="1" ht="95.25" customHeight="1" outlineLevel="1">
-      <c r="A66" s="223" t="s">
+      <c r="J65" s="166"/>
+    </row>
+    <row r="66" spans="1:10" s="162" customFormat="1" ht="95.25" customHeight="1" outlineLevel="1">
+      <c r="A66" s="163" t="s">
         <v>204</v>
       </c>
-      <c r="B66" s="207" t="s">
+      <c r="B66" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C66" s="208" t="s">
+      <c r="C66" s="151" t="s">
         <v>205</v>
       </c>
-      <c r="D66" s="227" t="s">
+      <c r="D66" s="181" t="s">
         <v>128</v>
       </c>
-      <c r="E66" s="228"/>
-      <c r="F66" s="228"/>
-      <c r="G66" s="224"/>
-      <c r="H66" s="214">
+      <c r="E66" s="182"/>
+      <c r="F66" s="182"/>
+      <c r="G66" s="164"/>
+      <c r="H66" s="155">
         <v>43774</v>
       </c>
-      <c r="I66" s="229" t="s">
+      <c r="I66" s="167" t="s">
         <v>8</v>
       </c>
-      <c r="J66" s="226"/>
-    </row>
-    <row r="67" spans="1:10" s="222" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
-      <c r="A67" s="223" t="s">
+      <c r="J66" s="166"/>
+    </row>
+    <row r="67" spans="1:10" s="162" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
+      <c r="A67" s="163" t="s">
         <v>206</v>
       </c>
-      <c r="B67" s="207" t="s">
+      <c r="B67" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C67" s="208" t="s">
+      <c r="C67" s="151" t="s">
         <v>207</v>
       </c>
-      <c r="D67" s="227" t="s">
+      <c r="D67" s="181" t="s">
         <v>128</v>
       </c>
-      <c r="E67" s="228"/>
-      <c r="F67" s="228"/>
-      <c r="G67" s="224"/>
-      <c r="H67" s="214">
+      <c r="E67" s="182"/>
+      <c r="F67" s="182"/>
+      <c r="G67" s="164"/>
+      <c r="H67" s="155">
         <v>43774</v>
       </c>
-      <c r="I67" s="229" t="s">
+      <c r="I67" s="167" t="s">
         <v>8</v>
       </c>
-      <c r="J67" s="226"/>
-    </row>
-    <row r="68" spans="1:10" s="222" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
-      <c r="A68" s="223" t="s">
+      <c r="J67" s="166"/>
+    </row>
+    <row r="68" spans="1:10" s="162" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
+      <c r="A68" s="163" t="s">
         <v>208</v>
       </c>
-      <c r="B68" s="207" t="s">
+      <c r="B68" s="150" t="s">
         <v>193</v>
       </c>
-      <c r="C68" s="208" t="s">
+      <c r="C68" s="151" t="s">
         <v>209</v>
       </c>
-      <c r="D68" s="227" t="s">
+      <c r="D68" s="181" t="s">
         <v>128</v>
       </c>
-      <c r="E68" s="228"/>
-      <c r="F68" s="228"/>
-      <c r="G68" s="224"/>
-      <c r="H68" s="214">
+      <c r="E68" s="182"/>
+      <c r="F68" s="182"/>
+      <c r="G68" s="164"/>
+      <c r="H68" s="155">
         <v>43774</v>
       </c>
-      <c r="I68" s="229" t="s">
+      <c r="I68" s="167" t="s">
         <v>8</v>
       </c>
-      <c r="J68" s="226"/>
-    </row>
-    <row r="69" spans="1:10" s="222" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
-      <c r="A69" s="218" t="s">
+      <c r="J68" s="166"/>
+    </row>
+    <row r="69" spans="1:10" s="162" customFormat="1" ht="93" customHeight="1" outlineLevel="1">
+      <c r="A69" s="158" t="s">
         <v>210</v>
       </c>
       <c r="B69" s="116" t="s">
@@ -7168,69 +7176,69 @@
       <c r="C69" s="117" t="s">
         <v>211</v>
       </c>
-      <c r="D69" s="230" t="s">
+      <c r="D69" s="183" t="s">
         <v>128</v>
       </c>
-      <c r="E69" s="231"/>
-      <c r="F69" s="231"/>
-      <c r="G69" s="219"/>
+      <c r="E69" s="184"/>
+      <c r="F69" s="184"/>
+      <c r="G69" s="159"/>
       <c r="H69" s="121">
         <v>43774</v>
       </c>
-      <c r="I69" s="220" t="s">
+      <c r="I69" s="160" t="s">
         <v>8</v>
       </c>
-      <c r="J69" s="221" t="s">
+      <c r="J69" s="161" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="212" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A70" s="206" t="s">
+    <row r="70" spans="1:10" s="154" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A70" s="149" t="s">
         <v>213</v>
       </c>
-      <c r="B70" s="207" t="s">
+      <c r="B70" s="150" t="s">
         <v>106</v>
       </c>
-      <c r="C70" s="208" t="s">
+      <c r="C70" s="151" t="s">
         <v>98</v>
       </c>
-      <c r="D70" s="213" t="s">
+      <c r="D70" s="175" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="209"/>
-      <c r="F70" s="209"/>
-      <c r="G70" s="210"/>
-      <c r="H70" s="214">
+      <c r="E70" s="176"/>
+      <c r="F70" s="176"/>
+      <c r="G70" s="152"/>
+      <c r="H70" s="155">
         <v>43774</v>
       </c>
       <c r="I70" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="J70" s="211"/>
-    </row>
-    <row r="71" spans="1:10" s="212" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
-      <c r="A71" s="206" t="s">
+      <c r="J70" s="153"/>
+    </row>
+    <row r="71" spans="1:10" s="154" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
+      <c r="A71" s="149" t="s">
         <v>214</v>
       </c>
-      <c r="B71" s="207" t="s">
+      <c r="B71" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="C71" s="208" t="s">
+      <c r="C71" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="D71" s="213" t="s">
+      <c r="D71" s="175" t="s">
         <v>107</v>
       </c>
-      <c r="E71" s="209"/>
-      <c r="F71" s="209"/>
-      <c r="G71" s="210"/>
-      <c r="H71" s="214">
+      <c r="E71" s="176"/>
+      <c r="F71" s="176"/>
+      <c r="G71" s="152"/>
+      <c r="H71" s="155">
         <v>43774</v>
       </c>
       <c r="I71" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J71" s="211"/>
+      <c r="J71" s="153"/>
     </row>
     <row r="72" spans="1:10" s="4" customFormat="1" ht="32.25" customHeight="1" outlineLevel="1">
       <c r="A72" s="88" t="s">
@@ -7242,11 +7250,11 @@
       <c r="C72" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="D72" s="162" t="s">
+      <c r="D72" s="178" t="s">
         <v>101</v>
       </c>
-      <c r="E72" s="163"/>
-      <c r="F72" s="163"/>
+      <c r="E72" s="179"/>
+      <c r="F72" s="179"/>
       <c r="G72" s="86"/>
       <c r="H72" s="123">
         <v>43774</v>
@@ -7266,11 +7274,11 @@
       <c r="C73" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="D73" s="162" t="s">
+      <c r="D73" s="178" t="s">
         <v>117</v>
       </c>
-      <c r="E73" s="163"/>
-      <c r="F73" s="163"/>
+      <c r="E73" s="179"/>
+      <c r="F73" s="179"/>
       <c r="G73" s="86"/>
       <c r="H73" s="122">
         <v>43774</v>
@@ -7290,11 +7298,11 @@
       <c r="C74" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="D74" s="162" t="s">
+      <c r="D74" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="E74" s="163"/>
-      <c r="F74" s="163"/>
+      <c r="E74" s="179"/>
+      <c r="F74" s="179"/>
       <c r="G74" s="86"/>
       <c r="H74" s="122">
         <v>43774</v>
@@ -7314,11 +7322,11 @@
       <c r="C75" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="D75" s="162" t="s">
+      <c r="D75" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="E75" s="163"/>
-      <c r="F75" s="199"/>
+      <c r="E75" s="179"/>
+      <c r="F75" s="180"/>
       <c r="G75" s="87"/>
       <c r="H75" s="122">
         <v>43774</v>
@@ -7338,11 +7346,11 @@
       <c r="C76" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="D76" s="162" t="s">
+      <c r="D76" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="E76" s="163"/>
-      <c r="F76" s="199"/>
+      <c r="E76" s="179"/>
+      <c r="F76" s="180"/>
       <c r="G76" s="124"/>
       <c r="H76" s="122">
         <v>43774</v>
@@ -7362,11 +7370,11 @@
       <c r="C77" s="103" t="s">
         <v>222</v>
       </c>
-      <c r="D77" s="162" t="s">
+      <c r="D77" s="178" t="s">
         <v>101</v>
       </c>
-      <c r="E77" s="163"/>
-      <c r="F77" s="199"/>
+      <c r="E77" s="179"/>
+      <c r="F77" s="180"/>
       <c r="G77" s="124"/>
       <c r="H77" s="122">
         <v>43774</v>
@@ -7386,11 +7394,11 @@
       <c r="C78" s="103" t="s">
         <v>223</v>
       </c>
-      <c r="D78" s="162" t="s">
+      <c r="D78" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="E78" s="163"/>
-      <c r="F78" s="199"/>
+      <c r="E78" s="179"/>
+      <c r="F78" s="180"/>
       <c r="G78" s="124"/>
       <c r="H78" s="122">
         <v>43774</v>
@@ -7410,11 +7418,11 @@
       <c r="C79" s="103" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="162" t="s">
+      <c r="D79" s="178" t="s">
         <v>226</v>
       </c>
-      <c r="E79" s="163"/>
-      <c r="F79" s="199"/>
+      <c r="E79" s="179"/>
+      <c r="F79" s="180"/>
       <c r="G79" s="124"/>
       <c r="H79" s="122">
         <v>43774</v>
@@ -7434,11 +7442,11 @@
       <c r="C80" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="D80" s="162" t="s">
+      <c r="D80" s="178" t="s">
         <v>231</v>
       </c>
-      <c r="E80" s="163"/>
-      <c r="F80" s="199"/>
+      <c r="E80" s="179"/>
+      <c r="F80" s="180"/>
       <c r="G80" s="87"/>
       <c r="H80" s="122">
         <v>43774</v>
@@ -7458,11 +7466,11 @@
       <c r="C81" s="103" t="s">
         <v>230</v>
       </c>
-      <c r="D81" s="162" t="s">
+      <c r="D81" s="178" t="s">
         <v>232</v>
       </c>
-      <c r="E81" s="163"/>
-      <c r="F81" s="199"/>
+      <c r="E81" s="179"/>
+      <c r="F81" s="180"/>
       <c r="G81" s="124"/>
       <c r="H81" s="123">
         <v>43774</v>
@@ -7482,11 +7490,11 @@
       <c r="C82" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="D82" s="162" t="s">
+      <c r="D82" s="178" t="s">
         <v>232</v>
       </c>
-      <c r="E82" s="163"/>
-      <c r="F82" s="199"/>
+      <c r="E82" s="179"/>
+      <c r="F82" s="180"/>
       <c r="G82" s="124"/>
       <c r="H82" s="123">
         <v>43774</v>
@@ -7506,11 +7514,11 @@
       <c r="C83" s="103" t="s">
         <v>238</v>
       </c>
-      <c r="D83" s="162" t="s">
+      <c r="D83" s="178" t="s">
         <v>232</v>
       </c>
-      <c r="E83" s="163"/>
-      <c r="F83" s="199"/>
+      <c r="E83" s="179"/>
+      <c r="F83" s="180"/>
       <c r="G83" s="124"/>
       <c r="H83" s="123">
         <v>43774</v>
@@ -7530,11 +7538,11 @@
       <c r="C84" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="D84" s="162" t="s">
+      <c r="D84" s="178" t="s">
         <v>232</v>
       </c>
-      <c r="E84" s="163"/>
-      <c r="F84" s="199"/>
+      <c r="E84" s="179"/>
+      <c r="F84" s="180"/>
       <c r="G84" s="124"/>
       <c r="H84" s="123">
         <v>43774</v>
@@ -7554,11 +7562,11 @@
       <c r="C85" s="103" t="s">
         <v>240</v>
       </c>
-      <c r="D85" s="162" t="s">
+      <c r="D85" s="178" t="s">
         <v>241</v>
       </c>
-      <c r="E85" s="163"/>
-      <c r="F85" s="199"/>
+      <c r="E85" s="179"/>
+      <c r="F85" s="180"/>
       <c r="G85" s="124"/>
       <c r="H85" s="123">
         <v>43774</v>
@@ -7578,11 +7586,11 @@
       <c r="C86" s="124" t="s">
         <v>243</v>
       </c>
-      <c r="D86" s="162" t="s">
+      <c r="D86" s="178" t="s">
         <v>249</v>
       </c>
-      <c r="E86" s="163"/>
-      <c r="F86" s="199"/>
+      <c r="E86" s="179"/>
+      <c r="F86" s="180"/>
       <c r="G86" s="124"/>
       <c r="H86" s="123">
         <v>43774</v>
@@ -7604,11 +7612,11 @@
       <c r="C87" s="124" t="s">
         <v>246</v>
       </c>
-      <c r="D87" s="162" t="s">
+      <c r="D87" s="178" t="s">
         <v>248</v>
       </c>
-      <c r="E87" s="163"/>
-      <c r="F87" s="199"/>
+      <c r="E87" s="179"/>
+      <c r="F87" s="180"/>
       <c r="G87" s="124"/>
       <c r="H87" s="123">
         <v>43774</v>
@@ -7628,11 +7636,11 @@
       <c r="C88" s="124" t="s">
         <v>247</v>
       </c>
-      <c r="D88" s="162" t="s">
+      <c r="D88" s="178" t="s">
         <v>248</v>
       </c>
-      <c r="E88" s="163"/>
-      <c r="F88" s="199"/>
+      <c r="E88" s="179"/>
+      <c r="F88" s="180"/>
       <c r="G88" s="124"/>
       <c r="H88" s="123">
         <v>43774</v>
@@ -7652,11 +7660,11 @@
       <c r="C89" s="124" t="s">
         <v>250</v>
       </c>
-      <c r="D89" s="162" t="s">
+      <c r="D89" s="178" t="s">
         <v>248</v>
       </c>
-      <c r="E89" s="163"/>
-      <c r="F89" s="199"/>
+      <c r="E89" s="179"/>
+      <c r="F89" s="180"/>
       <c r="G89" s="124"/>
       <c r="H89" s="123">
         <v>43774</v>
@@ -7676,11 +7684,11 @@
       <c r="C90" s="124" t="s">
         <v>252</v>
       </c>
-      <c r="D90" s="162" t="s">
+      <c r="D90" s="178" t="s">
         <v>248</v>
       </c>
-      <c r="E90" s="163"/>
-      <c r="F90" s="199"/>
+      <c r="E90" s="179"/>
+      <c r="F90" s="180"/>
       <c r="G90" s="124"/>
       <c r="H90" s="123">
         <v>43774</v>
@@ -7700,11 +7708,11 @@
       <c r="C91" s="124" t="s">
         <v>254</v>
       </c>
-      <c r="D91" s="162" t="s">
+      <c r="D91" s="178" t="s">
         <v>248</v>
       </c>
-      <c r="E91" s="163"/>
-      <c r="F91" s="199"/>
+      <c r="E91" s="179"/>
+      <c r="F91" s="180"/>
       <c r="G91" s="124"/>
       <c r="H91" s="123">
         <v>43774</v>
@@ -7724,11 +7732,11 @@
       <c r="C92" s="124" t="s">
         <v>256</v>
       </c>
-      <c r="D92" s="162" t="s">
+      <c r="D92" s="178" t="s">
         <v>249</v>
       </c>
-      <c r="E92" s="163"/>
-      <c r="F92" s="199"/>
+      <c r="E92" s="179"/>
+      <c r="F92" s="180"/>
       <c r="G92" s="124"/>
       <c r="H92" s="123">
         <v>43774</v>
@@ -7748,11 +7756,11 @@
       <c r="C93" s="124" t="s">
         <v>258</v>
       </c>
-      <c r="D93" s="162" t="s">
+      <c r="D93" s="178" t="s">
         <v>249</v>
       </c>
-      <c r="E93" s="163"/>
-      <c r="F93" s="199"/>
+      <c r="E93" s="179"/>
+      <c r="F93" s="180"/>
       <c r="G93" s="124"/>
       <c r="H93" s="123">
         <v>43774</v>
@@ -7772,13 +7780,13 @@
       <c r="C94" s="119" t="s">
         <v>260</v>
       </c>
-      <c r="D94" s="215" t="s">
+      <c r="D94" s="172" t="s">
         <v>248</v>
       </c>
-      <c r="E94" s="176"/>
-      <c r="F94" s="232"/>
+      <c r="E94" s="173"/>
+      <c r="F94" s="174"/>
       <c r="G94" s="119"/>
-      <c r="H94" s="233">
+      <c r="H94" s="168">
         <v>43774</v>
       </c>
       <c r="I94" s="119" t="s">
@@ -7789,74 +7797,74 @@
       </c>
     </row>
     <row r="95" spans="1:10" s="4" customFormat="1" ht="84.75" customHeight="1" outlineLevel="1">
-      <c r="A95" s="206" t="s">
+      <c r="A95" s="149" t="s">
         <v>262</v>
       </c>
-      <c r="B95" s="207" t="s">
+      <c r="B95" s="150" t="s">
         <v>125</v>
       </c>
       <c r="C95" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="D95" s="213" t="s">
+      <c r="D95" s="175" t="s">
         <v>248</v>
       </c>
-      <c r="E95" s="209"/>
-      <c r="F95" s="234"/>
+      <c r="E95" s="176"/>
+      <c r="F95" s="177"/>
       <c r="G95" s="112"/>
-      <c r="H95" s="235">
+      <c r="H95" s="169">
         <v>43774</v>
       </c>
       <c r="I95" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J95" s="211"/>
+      <c r="J95" s="153"/>
     </row>
     <row r="96" spans="1:10" s="4" customFormat="1" ht="84.75" customHeight="1" outlineLevel="1">
-      <c r="A96" s="206" t="s">
+      <c r="A96" s="149" t="s">
         <v>264</v>
       </c>
-      <c r="B96" s="207" t="s">
+      <c r="B96" s="150" t="s">
         <v>125</v>
       </c>
       <c r="C96" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D96" s="213" t="s">
+      <c r="D96" s="175" t="s">
         <v>248</v>
       </c>
-      <c r="E96" s="209"/>
-      <c r="F96" s="234"/>
+      <c r="E96" s="176"/>
+      <c r="F96" s="177"/>
       <c r="G96" s="112"/>
-      <c r="H96" s="235">
+      <c r="H96" s="169">
         <v>43774</v>
       </c>
       <c r="I96" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="J96" s="211"/>
+      <c r="J96" s="153"/>
     </row>
     <row r="97" spans="1:14" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A97" s="196" t="s">
+      <c r="A97" s="185" t="s">
         <v>104</v>
       </c>
-      <c r="B97" s="197"/>
-      <c r="C97" s="197"/>
-      <c r="D97" s="197"/>
-      <c r="E97" s="197"/>
-      <c r="F97" s="197"/>
-      <c r="G97" s="197"/>
-      <c r="H97" s="197"/>
-      <c r="I97" s="197"/>
-      <c r="J97" s="198"/>
+      <c r="B97" s="186"/>
+      <c r="C97" s="186"/>
+      <c r="D97" s="186"/>
+      <c r="E97" s="186"/>
+      <c r="F97" s="186"/>
+      <c r="G97" s="186"/>
+      <c r="H97" s="186"/>
+      <c r="I97" s="186"/>
+      <c r="J97" s="187"/>
     </row>
     <row r="98" spans="1:14" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A98" s="88"/>
       <c r="B98" s="102"/>
       <c r="C98" s="103"/>
-      <c r="D98" s="195"/>
-      <c r="E98" s="163"/>
-      <c r="F98" s="163"/>
+      <c r="D98" s="196"/>
+      <c r="E98" s="179"/>
+      <c r="F98" s="179"/>
       <c r="G98" s="86"/>
       <c r="H98" s="135"/>
       <c r="I98" s="87"/>
@@ -7866,9 +7874,9 @@
       <c r="A99" s="88"/>
       <c r="B99" s="102"/>
       <c r="C99" s="103"/>
-      <c r="D99" s="195"/>
-      <c r="E99" s="163"/>
-      <c r="F99" s="163"/>
+      <c r="D99" s="196"/>
+      <c r="E99" s="179"/>
+      <c r="F99" s="179"/>
       <c r="G99" s="86"/>
       <c r="H99" s="135"/>
       <c r="I99" s="87"/>
@@ -7878,9 +7886,9 @@
       <c r="A100" s="88"/>
       <c r="B100" s="102"/>
       <c r="C100" s="103"/>
-      <c r="D100" s="195"/>
-      <c r="E100" s="163"/>
-      <c r="F100" s="163"/>
+      <c r="D100" s="196"/>
+      <c r="E100" s="179"/>
+      <c r="F100" s="179"/>
       <c r="G100" s="86"/>
       <c r="H100" s="136"/>
       <c r="I100" s="87"/>
@@ -7890,27 +7898,27 @@
       <c r="A101" s="88"/>
       <c r="B101" s="102"/>
       <c r="C101" s="103"/>
-      <c r="D101" s="195"/>
-      <c r="E101" s="163"/>
-      <c r="F101" s="163"/>
+      <c r="D101" s="196"/>
+      <c r="E101" s="179"/>
+      <c r="F101" s="179"/>
       <c r="G101" s="86"/>
       <c r="H101" s="135"/>
       <c r="I101" s="87"/>
       <c r="J101" s="85"/>
     </row>
     <row r="102" spans="1:14" s="4" customFormat="1" ht="12.75">
-      <c r="A102" s="196" t="s">
+      <c r="A102" s="185" t="s">
         <v>110</v>
       </c>
-      <c r="B102" s="197"/>
-      <c r="C102" s="197"/>
-      <c r="D102" s="197"/>
-      <c r="E102" s="197"/>
-      <c r="F102" s="197"/>
-      <c r="G102" s="197"/>
-      <c r="H102" s="197"/>
-      <c r="I102" s="197"/>
-      <c r="J102" s="198"/>
+      <c r="B102" s="186"/>
+      <c r="C102" s="186"/>
+      <c r="D102" s="186"/>
+      <c r="E102" s="186"/>
+      <c r="F102" s="186"/>
+      <c r="G102" s="186"/>
+      <c r="H102" s="186"/>
+      <c r="I102" s="186"/>
+      <c r="J102" s="187"/>
     </row>
     <row r="103" spans="1:14" s="93" customFormat="1" ht="62.25" customHeight="1" outlineLevel="1">
       <c r="A103" s="88" t="s">
@@ -7922,11 +7930,11 @@
       <c r="C103" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="D103" s="200" t="s">
+      <c r="D103" s="188" t="s">
         <v>112</v>
       </c>
-      <c r="E103" s="200"/>
-      <c r="F103" s="200"/>
+      <c r="E103" s="188"/>
+      <c r="F103" s="188"/>
       <c r="G103" s="130"/>
       <c r="H103" s="137">
         <v>43774</v>
@@ -7946,11 +7954,11 @@
       <c r="C104" s="126" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="204" t="s">
+      <c r="D104" s="191" t="s">
         <v>103</v>
       </c>
-      <c r="E104" s="205"/>
-      <c r="F104" s="205"/>
+      <c r="E104" s="192"/>
+      <c r="F104" s="192"/>
       <c r="G104" s="131"/>
       <c r="H104" s="141">
         <v>43774</v>
@@ -7960,57 +7968,57 @@
       </c>
       <c r="J104" s="128"/>
     </row>
-    <row r="105" spans="1:14" s="148" customFormat="1" ht="78" customHeight="1" outlineLevel="1">
-      <c r="A105" s="115" t="s">
+    <row r="105" spans="1:14" s="235" customFormat="1" ht="78" customHeight="1" outlineLevel="1">
+      <c r="A105" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="B105" s="142" t="s">
+      <c r="B105" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="C105" s="143" t="s">
+      <c r="C105" s="227" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="175" t="s">
+      <c r="D105" s="228" t="s">
         <v>119</v>
       </c>
-      <c r="E105" s="203"/>
-      <c r="F105" s="203"/>
-      <c r="G105" s="144"/>
-      <c r="H105" s="149">
+      <c r="E105" s="229"/>
+      <c r="F105" s="229"/>
+      <c r="G105" s="230"/>
+      <c r="H105" s="231">
         <v>43774</v>
       </c>
-      <c r="I105" s="145" t="s">
-        <v>8</v>
-      </c>
-      <c r="J105" s="146"/>
-      <c r="K105" s="147"/>
-      <c r="L105" s="147"/>
-      <c r="M105" s="147"/>
-      <c r="N105" s="147"/>
+      <c r="I105" s="232" t="s">
+        <v>37</v>
+      </c>
+      <c r="J105" s="233"/>
+      <c r="K105" s="234"/>
+      <c r="L105" s="234"/>
+      <c r="M105" s="234"/>
+      <c r="N105" s="234"/>
     </row>
     <row r="106" spans="1:14" s="93" customFormat="1" ht="80.25" customHeight="1" outlineLevel="1">
-      <c r="A106" s="151" t="s">
+      <c r="A106" s="143" t="s">
         <v>47</v>
       </c>
-      <c r="B106" s="152" t="s">
+      <c r="B106" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="C106" s="153" t="s">
+      <c r="C106" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="D106" s="201" t="s">
+      <c r="D106" s="189" t="s">
         <v>121</v>
       </c>
-      <c r="E106" s="202"/>
-      <c r="F106" s="202"/>
+      <c r="E106" s="190"/>
+      <c r="F106" s="190"/>
       <c r="G106" s="131"/>
-      <c r="H106" s="154">
+      <c r="H106" s="146">
         <v>43774</v>
       </c>
-      <c r="I106" s="155" t="s">
+      <c r="I106" s="147" t="s">
         <v>37</v>
       </c>
-      <c r="J106" s="156"/>
+      <c r="J106" s="148"/>
     </row>
     <row r="107" spans="1:14" s="93" customFormat="1" ht="80.25" customHeight="1" outlineLevel="1">
       <c r="A107" s="88" t="s">
@@ -8019,54 +8027,54 @@
       <c r="B107" s="129" t="s">
         <v>120</v>
       </c>
-      <c r="C107" s="153" t="s">
+      <c r="C107" s="145" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="162" t="s">
+      <c r="D107" s="178" t="s">
         <v>124</v>
       </c>
-      <c r="E107" s="163"/>
-      <c r="F107" s="199"/>
+      <c r="E107" s="179"/>
+      <c r="F107" s="180"/>
       <c r="G107" s="130"/>
       <c r="H107" s="137"/>
-      <c r="I107" s="150"/>
+      <c r="I107" s="142"/>
       <c r="J107" s="94"/>
     </row>
     <row r="108" spans="1:14" s="4" customFormat="1" ht="12.75">
-      <c r="A108" s="159" t="s">
+      <c r="A108" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="B108" s="160"/>
-      <c r="C108" s="160"/>
-      <c r="D108" s="160"/>
-      <c r="E108" s="160"/>
-      <c r="F108" s="160"/>
-      <c r="G108" s="160"/>
-      <c r="H108" s="160"/>
-      <c r="I108" s="160"/>
-      <c r="J108" s="161"/>
+      <c r="B108" s="194"/>
+      <c r="C108" s="194"/>
+      <c r="D108" s="194"/>
+      <c r="E108" s="194"/>
+      <c r="F108" s="194"/>
+      <c r="G108" s="194"/>
+      <c r="H108" s="194"/>
+      <c r="I108" s="194"/>
+      <c r="J108" s="195"/>
     </row>
     <row r="109" spans="1:14" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A109" s="159" t="s">
+      <c r="A109" s="193" t="s">
         <v>59</v>
       </c>
-      <c r="B109" s="160"/>
-      <c r="C109" s="160"/>
-      <c r="D109" s="160"/>
-      <c r="E109" s="160"/>
-      <c r="F109" s="160"/>
-      <c r="G109" s="160"/>
-      <c r="H109" s="160"/>
-      <c r="I109" s="160"/>
-      <c r="J109" s="161"/>
+      <c r="B109" s="194"/>
+      <c r="C109" s="194"/>
+      <c r="D109" s="194"/>
+      <c r="E109" s="194"/>
+      <c r="F109" s="194"/>
+      <c r="G109" s="194"/>
+      <c r="H109" s="194"/>
+      <c r="I109" s="194"/>
+      <c r="J109" s="195"/>
     </row>
     <row r="110" spans="1:14" s="93" customFormat="1" ht="70.5" customHeight="1" outlineLevel="1">
       <c r="A110" s="88"/>
       <c r="B110" s="97"/>
       <c r="C110" s="92"/>
-      <c r="D110" s="162"/>
-      <c r="E110" s="163"/>
-      <c r="F110" s="163"/>
+      <c r="D110" s="178"/>
+      <c r="E110" s="179"/>
+      <c r="F110" s="179"/>
       <c r="G110" s="131"/>
       <c r="H110" s="138"/>
       <c r="I110" s="100"/>
@@ -8076,9 +8084,9 @@
       <c r="A111" s="88"/>
       <c r="B111" s="97"/>
       <c r="C111" s="92"/>
-      <c r="D111" s="162"/>
-      <c r="E111" s="163"/>
-      <c r="F111" s="163"/>
+      <c r="D111" s="178"/>
+      <c r="E111" s="179"/>
+      <c r="F111" s="179"/>
       <c r="G111" s="131"/>
       <c r="H111" s="138"/>
       <c r="I111" s="100"/>
@@ -8088,9 +8096,9 @@
       <c r="A112" s="88"/>
       <c r="B112" s="97"/>
       <c r="C112" s="92"/>
-      <c r="D112" s="162"/>
-      <c r="E112" s="163"/>
-      <c r="F112" s="163"/>
+      <c r="D112" s="178"/>
+      <c r="E112" s="179"/>
+      <c r="F112" s="179"/>
       <c r="G112" s="131"/>
       <c r="H112" s="138"/>
       <c r="I112" s="100"/>
@@ -8100,9 +8108,9 @@
       <c r="A113" s="88"/>
       <c r="B113" s="97"/>
       <c r="C113" s="92"/>
-      <c r="D113" s="162"/>
-      <c r="E113" s="163"/>
-      <c r="F113" s="163"/>
+      <c r="D113" s="178"/>
+      <c r="E113" s="179"/>
+      <c r="F113" s="179"/>
       <c r="G113" s="131"/>
       <c r="H113" s="138"/>
       <c r="I113" s="100"/>
@@ -8112,9 +8120,9 @@
       <c r="A114" s="88"/>
       <c r="B114" s="97"/>
       <c r="C114" s="92"/>
-      <c r="D114" s="162"/>
-      <c r="E114" s="163"/>
-      <c r="F114" s="163"/>
+      <c r="D114" s="178"/>
+      <c r="E114" s="179"/>
+      <c r="F114" s="179"/>
       <c r="G114" s="131"/>
       <c r="H114" s="138"/>
       <c r="I114" s="100"/>
@@ -8124,9 +8132,9 @@
       <c r="A115" s="88"/>
       <c r="B115" s="97"/>
       <c r="C115" s="92"/>
-      <c r="D115" s="162"/>
-      <c r="E115" s="163"/>
-      <c r="F115" s="163"/>
+      <c r="D115" s="178"/>
+      <c r="E115" s="179"/>
+      <c r="F115" s="179"/>
       <c r="G115" s="131"/>
       <c r="H115" s="138"/>
       <c r="I115" s="100"/>
@@ -8136,61 +8144,61 @@
       <c r="A116" s="88"/>
       <c r="B116" s="97"/>
       <c r="C116" s="92"/>
-      <c r="D116" s="162"/>
-      <c r="E116" s="163"/>
-      <c r="F116" s="163"/>
+      <c r="D116" s="178"/>
+      <c r="E116" s="179"/>
+      <c r="F116" s="179"/>
       <c r="G116" s="131"/>
       <c r="H116" s="138"/>
       <c r="I116" s="100"/>
       <c r="J116" s="94"/>
     </row>
     <row r="117" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A117" s="159" t="s">
+      <c r="A117" s="193" t="s">
         <v>51</v>
       </c>
-      <c r="B117" s="160"/>
-      <c r="C117" s="160"/>
-      <c r="D117" s="160"/>
-      <c r="E117" s="160"/>
-      <c r="F117" s="160"/>
-      <c r="G117" s="160"/>
-      <c r="H117" s="160"/>
-      <c r="I117" s="160"/>
-      <c r="J117" s="161"/>
+      <c r="B117" s="194"/>
+      <c r="C117" s="194"/>
+      <c r="D117" s="194"/>
+      <c r="E117" s="194"/>
+      <c r="F117" s="194"/>
+      <c r="G117" s="194"/>
+      <c r="H117" s="194"/>
+      <c r="I117" s="194"/>
+      <c r="J117" s="195"/>
     </row>
     <row r="118" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A118" s="88"/>
       <c r="B118" s="97"/>
       <c r="C118" s="92"/>
-      <c r="D118" s="162"/>
-      <c r="E118" s="163"/>
-      <c r="F118" s="163"/>
+      <c r="D118" s="178"/>
+      <c r="E118" s="179"/>
+      <c r="F118" s="179"/>
       <c r="G118" s="131"/>
       <c r="H118" s="138"/>
       <c r="I118" s="100"/>
       <c r="J118" s="94"/>
     </row>
     <row r="119" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A119" s="159" t="s">
+      <c r="A119" s="193" t="s">
         <v>52</v>
       </c>
-      <c r="B119" s="160"/>
-      <c r="C119" s="160"/>
-      <c r="D119" s="160"/>
-      <c r="E119" s="160"/>
-      <c r="F119" s="160"/>
-      <c r="G119" s="160"/>
-      <c r="H119" s="160"/>
-      <c r="I119" s="160"/>
-      <c r="J119" s="161"/>
+      <c r="B119" s="194"/>
+      <c r="C119" s="194"/>
+      <c r="D119" s="194"/>
+      <c r="E119" s="194"/>
+      <c r="F119" s="194"/>
+      <c r="G119" s="194"/>
+      <c r="H119" s="194"/>
+      <c r="I119" s="194"/>
+      <c r="J119" s="195"/>
     </row>
     <row r="120" spans="1:10" s="93" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
       <c r="A120" s="88"/>
       <c r="B120" s="97"/>
       <c r="C120" s="92"/>
-      <c r="D120" s="162"/>
-      <c r="E120" s="163"/>
-      <c r="F120" s="163"/>
+      <c r="D120" s="178"/>
+      <c r="E120" s="179"/>
+      <c r="F120" s="179"/>
       <c r="G120" s="131"/>
       <c r="H120" s="138"/>
       <c r="I120" s="106"/>
@@ -8200,9 +8208,9 @@
       <c r="A121" s="88"/>
       <c r="B121" s="97"/>
       <c r="C121" s="92"/>
-      <c r="D121" s="162"/>
-      <c r="E121" s="163"/>
-      <c r="F121" s="163"/>
+      <c r="D121" s="178"/>
+      <c r="E121" s="179"/>
+      <c r="F121" s="179"/>
       <c r="G121" s="131"/>
       <c r="H121" s="138"/>
       <c r="I121" s="100"/>
@@ -8212,35 +8220,35 @@
       <c r="A122" s="88"/>
       <c r="B122" s="97"/>
       <c r="C122" s="92"/>
-      <c r="D122" s="162"/>
-      <c r="E122" s="163"/>
-      <c r="F122" s="163"/>
+      <c r="D122" s="178"/>
+      <c r="E122" s="179"/>
+      <c r="F122" s="179"/>
       <c r="G122" s="131"/>
       <c r="H122" s="138"/>
       <c r="I122" s="100"/>
       <c r="J122" s="94"/>
     </row>
     <row r="123" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A123" s="159" t="s">
+      <c r="A123" s="193" t="s">
         <v>53</v>
       </c>
-      <c r="B123" s="160"/>
-      <c r="C123" s="160"/>
-      <c r="D123" s="160"/>
-      <c r="E123" s="160"/>
-      <c r="F123" s="160"/>
-      <c r="G123" s="160"/>
-      <c r="H123" s="160"/>
-      <c r="I123" s="160"/>
-      <c r="J123" s="161"/>
+      <c r="B123" s="194"/>
+      <c r="C123" s="194"/>
+      <c r="D123" s="194"/>
+      <c r="E123" s="194"/>
+      <c r="F123" s="194"/>
+      <c r="G123" s="194"/>
+      <c r="H123" s="194"/>
+      <c r="I123" s="194"/>
+      <c r="J123" s="195"/>
     </row>
     <row r="124" spans="1:10" s="93" customFormat="1" ht="27.75" customHeight="1" outlineLevel="1">
       <c r="A124" s="88"/>
       <c r="B124" s="97"/>
       <c r="C124" s="92"/>
-      <c r="D124" s="162"/>
-      <c r="E124" s="163"/>
-      <c r="F124" s="163"/>
+      <c r="D124" s="178"/>
+      <c r="E124" s="179"/>
+      <c r="F124" s="179"/>
       <c r="G124" s="131"/>
       <c r="H124" s="138"/>
       <c r="I124" s="100"/>
@@ -8250,49 +8258,49 @@
       <c r="A125" s="88"/>
       <c r="B125" s="97"/>
       <c r="C125" s="92"/>
-      <c r="D125" s="164"/>
-      <c r="E125" s="163"/>
-      <c r="F125" s="163"/>
+      <c r="D125" s="225"/>
+      <c r="E125" s="179"/>
+      <c r="F125" s="179"/>
       <c r="G125" s="131"/>
       <c r="H125" s="138"/>
       <c r="I125" s="100"/>
       <c r="J125" s="94"/>
     </row>
     <row r="126" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A126" s="159" t="s">
+      <c r="A126" s="193" t="s">
         <v>54</v>
       </c>
-      <c r="B126" s="160"/>
-      <c r="C126" s="160"/>
-      <c r="D126" s="160"/>
-      <c r="E126" s="160"/>
-      <c r="F126" s="160"/>
-      <c r="G126" s="160"/>
-      <c r="H126" s="160"/>
-      <c r="I126" s="160"/>
-      <c r="J126" s="161"/>
+      <c r="B126" s="194"/>
+      <c r="C126" s="194"/>
+      <c r="D126" s="194"/>
+      <c r="E126" s="194"/>
+      <c r="F126" s="194"/>
+      <c r="G126" s="194"/>
+      <c r="H126" s="194"/>
+      <c r="I126" s="194"/>
+      <c r="J126" s="195"/>
     </row>
     <row r="127" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A127" s="159" t="s">
+      <c r="A127" s="193" t="s">
         <v>55</v>
       </c>
-      <c r="B127" s="160"/>
-      <c r="C127" s="160"/>
-      <c r="D127" s="160"/>
-      <c r="E127" s="160"/>
-      <c r="F127" s="160"/>
-      <c r="G127" s="160"/>
-      <c r="H127" s="160"/>
-      <c r="I127" s="160"/>
-      <c r="J127" s="161"/>
+      <c r="B127" s="194"/>
+      <c r="C127" s="194"/>
+      <c r="D127" s="194"/>
+      <c r="E127" s="194"/>
+      <c r="F127" s="194"/>
+      <c r="G127" s="194"/>
+      <c r="H127" s="194"/>
+      <c r="I127" s="194"/>
+      <c r="J127" s="195"/>
     </row>
     <row r="128" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A128" s="88"/>
       <c r="B128" s="97"/>
       <c r="C128" s="92"/>
-      <c r="D128" s="162"/>
-      <c r="E128" s="163"/>
-      <c r="F128" s="163"/>
+      <c r="D128" s="178"/>
+      <c r="E128" s="179"/>
+      <c r="F128" s="179"/>
       <c r="G128" s="131"/>
       <c r="H128" s="138"/>
       <c r="I128" s="100"/>
@@ -8302,35 +8310,35 @@
       <c r="A129" s="88"/>
       <c r="B129" s="97"/>
       <c r="C129" s="92"/>
-      <c r="D129" s="162"/>
-      <c r="E129" s="163"/>
-      <c r="F129" s="163"/>
+      <c r="D129" s="178"/>
+      <c r="E129" s="179"/>
+      <c r="F129" s="179"/>
       <c r="G129" s="131"/>
       <c r="H129" s="138"/>
       <c r="I129" s="100"/>
       <c r="J129" s="94"/>
     </row>
     <row r="130" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A130" s="159" t="s">
+      <c r="A130" s="193" t="s">
         <v>56</v>
       </c>
-      <c r="B130" s="160"/>
-      <c r="C130" s="160"/>
-      <c r="D130" s="160"/>
-      <c r="E130" s="160"/>
-      <c r="F130" s="160"/>
-      <c r="G130" s="160"/>
-      <c r="H130" s="160"/>
-      <c r="I130" s="160"/>
-      <c r="J130" s="161"/>
+      <c r="B130" s="194"/>
+      <c r="C130" s="194"/>
+      <c r="D130" s="194"/>
+      <c r="E130" s="194"/>
+      <c r="F130" s="194"/>
+      <c r="G130" s="194"/>
+      <c r="H130" s="194"/>
+      <c r="I130" s="194"/>
+      <c r="J130" s="195"/>
     </row>
     <row r="131" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A131" s="88"/>
       <c r="B131" s="97"/>
       <c r="C131" s="92"/>
-      <c r="D131" s="162"/>
-      <c r="E131" s="163"/>
-      <c r="F131" s="163"/>
+      <c r="D131" s="178"/>
+      <c r="E131" s="179"/>
+      <c r="F131" s="179"/>
       <c r="G131" s="131"/>
       <c r="H131" s="138"/>
       <c r="I131" s="100"/>
@@ -8340,35 +8348,35 @@
       <c r="A132" s="88"/>
       <c r="B132" s="97"/>
       <c r="C132" s="92"/>
-      <c r="D132" s="162"/>
-      <c r="E132" s="163"/>
-      <c r="F132" s="163"/>
+      <c r="D132" s="178"/>
+      <c r="E132" s="179"/>
+      <c r="F132" s="179"/>
       <c r="G132" s="131"/>
       <c r="H132" s="138"/>
       <c r="I132" s="100"/>
       <c r="J132" s="94"/>
     </row>
     <row r="133" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A133" s="159" t="s">
+      <c r="A133" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="B133" s="160"/>
-      <c r="C133" s="160"/>
-      <c r="D133" s="160"/>
-      <c r="E133" s="160"/>
-      <c r="F133" s="160"/>
-      <c r="G133" s="160"/>
-      <c r="H133" s="160"/>
-      <c r="I133" s="160"/>
-      <c r="J133" s="161"/>
+      <c r="B133" s="194"/>
+      <c r="C133" s="194"/>
+      <c r="D133" s="194"/>
+      <c r="E133" s="194"/>
+      <c r="F133" s="194"/>
+      <c r="G133" s="194"/>
+      <c r="H133" s="194"/>
+      <c r="I133" s="194"/>
+      <c r="J133" s="195"/>
     </row>
     <row r="134" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A134" s="88"/>
       <c r="B134" s="97"/>
       <c r="C134" s="92"/>
-      <c r="D134" s="162"/>
-      <c r="E134" s="163"/>
-      <c r="F134" s="163"/>
+      <c r="D134" s="178"/>
+      <c r="E134" s="179"/>
+      <c r="F134" s="179"/>
       <c r="G134" s="131"/>
       <c r="H134" s="138"/>
       <c r="I134" s="100"/>
@@ -8378,35 +8386,35 @@
       <c r="A135" s="88"/>
       <c r="B135" s="97"/>
       <c r="C135" s="92"/>
-      <c r="D135" s="162"/>
-      <c r="E135" s="163"/>
-      <c r="F135" s="163"/>
+      <c r="D135" s="178"/>
+      <c r="E135" s="179"/>
+      <c r="F135" s="179"/>
       <c r="G135" s="131"/>
       <c r="H135" s="138"/>
       <c r="I135" s="100"/>
       <c r="J135" s="94"/>
     </row>
     <row r="136" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A136" s="159" t="s">
+      <c r="A136" s="193" t="s">
         <v>58</v>
       </c>
-      <c r="B136" s="160"/>
-      <c r="C136" s="160"/>
-      <c r="D136" s="160"/>
-      <c r="E136" s="160"/>
-      <c r="F136" s="160"/>
-      <c r="G136" s="160"/>
-      <c r="H136" s="160"/>
-      <c r="I136" s="160"/>
-      <c r="J136" s="161"/>
+      <c r="B136" s="194"/>
+      <c r="C136" s="194"/>
+      <c r="D136" s="194"/>
+      <c r="E136" s="194"/>
+      <c r="F136" s="194"/>
+      <c r="G136" s="194"/>
+      <c r="H136" s="194"/>
+      <c r="I136" s="194"/>
+      <c r="J136" s="195"/>
     </row>
     <row r="137" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A137" s="88"/>
       <c r="B137" s="97"/>
       <c r="C137" s="92"/>
-      <c r="D137" s="162"/>
-      <c r="E137" s="163"/>
-      <c r="F137" s="163"/>
+      <c r="D137" s="178"/>
+      <c r="E137" s="179"/>
+      <c r="F137" s="179"/>
       <c r="G137" s="131"/>
       <c r="H137" s="138"/>
       <c r="I137" s="100"/>
@@ -8416,35 +8424,35 @@
       <c r="A138" s="88"/>
       <c r="B138" s="97"/>
       <c r="C138" s="92"/>
-      <c r="D138" s="162"/>
-      <c r="E138" s="163"/>
-      <c r="F138" s="163"/>
+      <c r="D138" s="178"/>
+      <c r="E138" s="179"/>
+      <c r="F138" s="179"/>
       <c r="G138" s="131"/>
       <c r="H138" s="138"/>
       <c r="I138" s="100"/>
       <c r="J138" s="94"/>
     </row>
     <row r="139" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A139" s="159" t="s">
+      <c r="A139" s="193" t="s">
         <v>61</v>
       </c>
-      <c r="B139" s="160"/>
-      <c r="C139" s="160"/>
-      <c r="D139" s="160"/>
-      <c r="E139" s="160"/>
-      <c r="F139" s="160"/>
-      <c r="G139" s="160"/>
-      <c r="H139" s="160"/>
-      <c r="I139" s="160"/>
-      <c r="J139" s="161"/>
+      <c r="B139" s="194"/>
+      <c r="C139" s="194"/>
+      <c r="D139" s="194"/>
+      <c r="E139" s="194"/>
+      <c r="F139" s="194"/>
+      <c r="G139" s="194"/>
+      <c r="H139" s="194"/>
+      <c r="I139" s="194"/>
+      <c r="J139" s="195"/>
     </row>
     <row r="140" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A140" s="88"/>
       <c r="B140" s="97"/>
       <c r="C140" s="92"/>
-      <c r="D140" s="162"/>
-      <c r="E140" s="163"/>
-      <c r="F140" s="163"/>
+      <c r="D140" s="178"/>
+      <c r="E140" s="179"/>
+      <c r="F140" s="179"/>
       <c r="G140" s="131"/>
       <c r="H140" s="138"/>
       <c r="I140" s="100"/>
@@ -8454,9 +8462,9 @@
       <c r="A141" s="88"/>
       <c r="B141" s="97"/>
       <c r="C141" s="92"/>
-      <c r="D141" s="162"/>
-      <c r="E141" s="163"/>
-      <c r="F141" s="163"/>
+      <c r="D141" s="178"/>
+      <c r="E141" s="179"/>
+      <c r="F141" s="179"/>
       <c r="G141" s="131"/>
       <c r="H141" s="138"/>
       <c r="I141" s="100"/>
@@ -8502,29 +8510,108 @@
     <row r="179" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="A139:J139"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D135:F135"/>
+    <mergeCell ref="A136:J136"/>
+    <mergeCell ref="D137:F137"/>
+    <mergeCell ref="D138:F138"/>
+    <mergeCell ref="D131:F131"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="A127:J127"/>
+    <mergeCell ref="A130:J130"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D115:F115"/>
+    <mergeCell ref="A123:J123"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="A133:J133"/>
+    <mergeCell ref="A126:J126"/>
+    <mergeCell ref="D124:F124"/>
+    <mergeCell ref="D125:F125"/>
+    <mergeCell ref="A117:J117"/>
+    <mergeCell ref="A119:J119"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="A109:J109"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="D99:F99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="A102:J102"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="A108:J108"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="A24:J24"/>
     <mergeCell ref="D52:F52"/>
     <mergeCell ref="D53:F53"/>
     <mergeCell ref="D54:F54"/>
@@ -8548,108 +8635,29 @@
     <mergeCell ref="D74:F74"/>
     <mergeCell ref="D72:F72"/>
     <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="A108:J108"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="A97:J97"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="A109:J109"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="D99:F99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="A102:J102"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D115:F115"/>
-    <mergeCell ref="A123:J123"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="A133:J133"/>
-    <mergeCell ref="A126:J126"/>
-    <mergeCell ref="D124:F124"/>
-    <mergeCell ref="D125:F125"/>
-    <mergeCell ref="A117:J117"/>
-    <mergeCell ref="A119:J119"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="A139:J139"/>
-    <mergeCell ref="D140:F140"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="D135:F135"/>
-    <mergeCell ref="A136:J136"/>
-    <mergeCell ref="D137:F137"/>
-    <mergeCell ref="D138:F138"/>
-    <mergeCell ref="D131:F131"/>
-    <mergeCell ref="D132:F132"/>
-    <mergeCell ref="D134:F134"/>
-    <mergeCell ref="D128:F128"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="A127:J127"/>
-    <mergeCell ref="A130:J130"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D77:F77"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8762,11 +8770,11 @@
       </c>
       <c r="D8" s="76">
         <f>'Export all carrier choices'!B6</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E8" s="75">
         <f>'Export all carrier choices'!B7</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="75">
         <f>'Export all carrier choices'!D6</f>
@@ -8794,11 +8802,11 @@
       </c>
       <c r="D10" s="61">
         <f>SUM(D6:D9)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" s="61">
         <f>SUM(E6:E9)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="61">
         <f>SUM(F6:F9)</f>
@@ -8843,7 +8851,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="24">
         <f>D10*100/G10</f>
-        <v>62.068965517241381</v>
+        <v>63.218390804597703</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Them chuc nang Thong ke doanh thu ahihi
</commit_message>
<xml_diff>
--- a/test-case.xlsx
+++ b/test-case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="300" windowWidth="12120" windowHeight="9060" tabRatio="821" activeTab="1"/>
+    <workbookView xWindow="1635" yWindow="750" windowWidth="12120" windowHeight="9060" tabRatio="821" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -2531,184 +2531,10 @@
     <xf numFmtId="14" fontId="25" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2725,6 +2551,180 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5400,11 +5400,11 @@
       <c r="B6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="170" t="s">
+      <c r="C6" s="178" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="170"/>
-      <c r="E6" s="171"/>
+      <c r="D6" s="178"/>
+      <c r="E6" s="179"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
     </row>
@@ -5413,11 +5413,11 @@
       <c r="B7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="170" t="s">
+      <c r="C7" s="178" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="170"/>
-      <c r="E7" s="171"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="179"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
     </row>
@@ -5630,8 +5630,8 @@
   </sheetPr>
   <dimension ref="A1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I105" sqref="I105"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -5650,9 +5650,9 @@
       <c r="A1" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -5663,9 +5663,9 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
+      <c r="B2" s="187"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -5678,51 +5678,51 @@
       <c r="A3" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="170" t="s">
+      <c r="B3" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="170"/>
-      <c r="D3" s="171"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="179"/>
       <c r="E3" s="68"/>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
-      <c r="H3" s="204"/>
-      <c r="I3" s="204"/>
-      <c r="J3" s="204"/>
+      <c r="H3" s="193"/>
+      <c r="I3" s="193"/>
+      <c r="J3" s="193"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" ht="12.75">
       <c r="A4" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="206" t="s">
+      <c r="B4" s="195" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="208"/>
+      <c r="C4" s="196"/>
+      <c r="D4" s="197"/>
       <c r="E4" s="68"/>
       <c r="F4" s="68"/>
       <c r="G4" s="68"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-      <c r="J4" s="204"/>
+      <c r="H4" s="193"/>
+      <c r="I4" s="193"/>
+      <c r="J4" s="193"/>
       <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" s="81" customFormat="1" ht="12.75">
       <c r="A5" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="200" t="s">
+      <c r="B5" s="189" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="201"/>
-      <c r="D5" s="202"/>
+      <c r="C5" s="190"/>
+      <c r="D5" s="191"/>
       <c r="E5" s="79"/>
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
-      <c r="H5" s="203"/>
-      <c r="I5" s="203"/>
-      <c r="J5" s="203"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="192"/>
       <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
@@ -5743,9 +5743,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="204"/>
-      <c r="I6" s="204"/>
-      <c r="J6" s="204"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="193"/>
+      <c r="J6" s="193"/>
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -5766,16 +5766,16 @@
       <c r="E7" s="69"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
-      <c r="H7" s="204"/>
-      <c r="I7" s="204"/>
-      <c r="J7" s="204"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="193"/>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="199"/>
-      <c r="B8" s="199"/>
-      <c r="C8" s="199"/>
-      <c r="D8" s="199"/>
+      <c r="A8" s="188"/>
+      <c r="B8" s="188"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="188"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
@@ -5785,70 +5785,70 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" s="83" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="213" t="s">
+      <c r="A9" s="202" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="214" t="s">
+      <c r="B9" s="203" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="213" t="s">
+      <c r="C9" s="202" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="216" t="s">
+      <c r="D9" s="205" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="217"/>
-      <c r="F9" s="217"/>
-      <c r="G9" s="218"/>
-      <c r="H9" s="209" t="s">
+      <c r="E9" s="206"/>
+      <c r="F9" s="206"/>
+      <c r="G9" s="207"/>
+      <c r="H9" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="205" t="s">
+      <c r="I9" s="194" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="205" t="s">
+      <c r="J9" s="194" t="s">
         <v>79</v>
       </c>
       <c r="K9" s="82"/>
     </row>
     <row r="10" spans="1:11" s="71" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="205"/>
-      <c r="B10" s="215"/>
-      <c r="C10" s="205"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="221"/>
-      <c r="H10" s="210"/>
-      <c r="I10" s="205"/>
-      <c r="J10" s="205"/>
+      <c r="A10" s="194"/>
+      <c r="B10" s="204"/>
+      <c r="C10" s="194"/>
+      <c r="D10" s="208"/>
+      <c r="E10" s="209"/>
+      <c r="F10" s="209"/>
+      <c r="G10" s="210"/>
+      <c r="H10" s="199"/>
+      <c r="I10" s="194"/>
+      <c r="J10" s="194"/>
       <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:11" s="84" customFormat="1" ht="15">
-      <c r="A11" s="211"/>
-      <c r="B11" s="211"/>
-      <c r="C11" s="211"/>
-      <c r="D11" s="211"/>
-      <c r="E11" s="211"/>
-      <c r="F11" s="211"/>
-      <c r="G11" s="211"/>
-      <c r="H11" s="211"/>
-      <c r="I11" s="211"/>
-      <c r="J11" s="212"/>
+      <c r="A11" s="200"/>
+      <c r="B11" s="200"/>
+      <c r="C11" s="200"/>
+      <c r="D11" s="200"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="201"/>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" ht="12.75">
-      <c r="A12" s="193" t="s">
+      <c r="A12" s="180" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="194"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
-      <c r="F12" s="194"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="194"/>
-      <c r="I12" s="194"/>
-      <c r="J12" s="195"/>
+      <c r="B12" s="181"/>
+      <c r="C12" s="181"/>
+      <c r="D12" s="181"/>
+      <c r="E12" s="181"/>
+      <c r="F12" s="181"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="181"/>
+      <c r="I12" s="181"/>
+      <c r="J12" s="182"/>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" ht="47.25" customHeight="1" outlineLevel="1">
       <c r="A13" s="88" t="s">
@@ -5860,11 +5860,11 @@
       <c r="C13" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="178" t="s">
+      <c r="D13" s="183" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="179"/>
-      <c r="F13" s="179"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="184"/>
       <c r="G13" s="86"/>
       <c r="H13" s="122">
         <v>43774</v>
@@ -5884,11 +5884,11 @@
       <c r="C14" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="178" t="s">
+      <c r="D14" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="179"/>
-      <c r="F14" s="179"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
       <c r="G14" s="86"/>
       <c r="H14" s="122">
         <v>43774</v>
@@ -5908,11 +5908,11 @@
       <c r="C15" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="178" t="s">
+      <c r="D15" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="179"/>
-      <c r="F15" s="179"/>
+      <c r="E15" s="184"/>
+      <c r="F15" s="184"/>
       <c r="G15" s="86"/>
       <c r="H15" s="122">
         <v>43774</v>
@@ -5932,11 +5932,11 @@
       <c r="C16" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="178" t="s">
+      <c r="D16" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="179"/>
-      <c r="F16" s="179"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
       <c r="G16" s="86"/>
       <c r="H16" s="122">
         <v>43774</v>
@@ -5956,11 +5956,11 @@
       <c r="C17" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="178" t="s">
+      <c r="D17" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="179"/>
-      <c r="F17" s="179"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="184"/>
       <c r="G17" s="86"/>
       <c r="H17" s="122">
         <v>43774</v>
@@ -5980,11 +5980,11 @@
       <c r="C18" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="178" t="s">
+      <c r="D18" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="179"/>
-      <c r="F18" s="179"/>
+      <c r="E18" s="184"/>
+      <c r="F18" s="184"/>
       <c r="G18" s="86"/>
       <c r="H18" s="122">
         <v>43774</v>
@@ -6004,11 +6004,11 @@
       <c r="C19" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="178" t="s">
+      <c r="D19" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="179"/>
-      <c r="F19" s="179"/>
+      <c r="E19" s="184"/>
+      <c r="F19" s="184"/>
       <c r="G19" s="86"/>
       <c r="H19" s="122">
         <v>43774</v>
@@ -6028,11 +6028,11 @@
       <c r="C20" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="178" t="s">
+      <c r="D20" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="179"/>
-      <c r="F20" s="179"/>
+      <c r="E20" s="184"/>
+      <c r="F20" s="184"/>
       <c r="G20" s="86"/>
       <c r="H20" s="122">
         <v>43774</v>
@@ -6052,11 +6052,11 @@
       <c r="C21" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="178" t="s">
+      <c r="D21" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="179"/>
-      <c r="F21" s="179"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="184"/>
       <c r="G21" s="86"/>
       <c r="H21" s="122">
         <v>43774</v>
@@ -6076,11 +6076,11 @@
       <c r="C22" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="178" t="s">
+      <c r="D22" s="183" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="179"/>
-      <c r="F22" s="179"/>
+      <c r="E22" s="184"/>
+      <c r="F22" s="184"/>
       <c r="G22" s="86"/>
       <c r="H22" s="122">
         <v>43774</v>
@@ -6100,11 +6100,11 @@
       <c r="C23" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="178" t="s">
+      <c r="D23" s="183" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="179"/>
-      <c r="F23" s="179"/>
+      <c r="E23" s="184"/>
+      <c r="F23" s="184"/>
       <c r="G23" s="86"/>
       <c r="H23" s="122">
         <v>43774</v>
@@ -6115,23 +6115,23 @@
       <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" ht="21.75" customHeight="1" outlineLevel="1">
-      <c r="A24" s="222"/>
-      <c r="B24" s="223"/>
-      <c r="C24" s="223"/>
-      <c r="D24" s="223"/>
-      <c r="E24" s="223"/>
-      <c r="F24" s="223"/>
-      <c r="G24" s="223"/>
-      <c r="H24" s="223"/>
-      <c r="I24" s="223"/>
-      <c r="J24" s="224"/>
+      <c r="A24" s="225"/>
+      <c r="B24" s="226"/>
+      <c r="C24" s="226"/>
+      <c r="D24" s="226"/>
+      <c r="E24" s="226"/>
+      <c r="F24" s="226"/>
+      <c r="G24" s="226"/>
+      <c r="H24" s="226"/>
+      <c r="I24" s="226"/>
+      <c r="J24" s="227"/>
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A25" s="193" t="s">
+      <c r="A25" s="180" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="194"/>
-      <c r="C25" s="194"/>
+      <c r="B25" s="181"/>
+      <c r="C25" s="181"/>
       <c r="D25" s="113"/>
       <c r="E25" s="113"/>
       <c r="F25" s="113"/>
@@ -6141,18 +6141,18 @@
       <c r="J25" s="114"/>
     </row>
     <row r="26" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A26" s="185" t="s">
+      <c r="A26" s="211" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="186"/>
-      <c r="C26" s="186"/>
-      <c r="D26" s="186"/>
-      <c r="E26" s="186"/>
-      <c r="F26" s="186"/>
-      <c r="G26" s="186"/>
-      <c r="H26" s="186"/>
-      <c r="I26" s="186"/>
-      <c r="J26" s="187"/>
+      <c r="B26" s="212"/>
+      <c r="C26" s="212"/>
+      <c r="D26" s="212"/>
+      <c r="E26" s="212"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="212"/>
+      <c r="H26" s="212"/>
+      <c r="I26" s="212"/>
+      <c r="J26" s="213"/>
     </row>
     <row r="27" spans="1:10" s="154" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
       <c r="A27" s="149" t="s">
@@ -6164,11 +6164,11 @@
       <c r="C27" s="151" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="175" t="s">
+      <c r="D27" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
+      <c r="E27" s="224"/>
+      <c r="F27" s="224"/>
       <c r="G27" s="152"/>
       <c r="H27" s="155">
         <v>43774</v>
@@ -6188,11 +6188,11 @@
       <c r="C28" s="151" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="175" t="s">
+      <c r="D28" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="176"/>
-      <c r="F28" s="176"/>
+      <c r="E28" s="224"/>
+      <c r="F28" s="224"/>
       <c r="G28" s="152"/>
       <c r="H28" s="155">
         <v>43774</v>
@@ -6212,11 +6212,11 @@
       <c r="C29" s="151" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="175" t="s">
+      <c r="D29" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="176"/>
-      <c r="F29" s="176"/>
+      <c r="E29" s="224"/>
+      <c r="F29" s="224"/>
       <c r="G29" s="152"/>
       <c r="H29" s="155">
         <v>43774</v>
@@ -6236,11 +6236,11 @@
       <c r="C30" s="151" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="175" t="s">
+      <c r="D30" s="223" t="s">
         <v>135</v>
       </c>
-      <c r="E30" s="176"/>
-      <c r="F30" s="176"/>
+      <c r="E30" s="224"/>
+      <c r="F30" s="224"/>
       <c r="G30" s="152"/>
       <c r="H30" s="155">
         <v>43774</v>
@@ -6260,11 +6260,11 @@
       <c r="C31" s="151" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="175" t="s">
+      <c r="D31" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E31" s="176"/>
-      <c r="F31" s="176"/>
+      <c r="E31" s="224"/>
+      <c r="F31" s="224"/>
       <c r="G31" s="152"/>
       <c r="H31" s="155">
         <v>43774</v>
@@ -6284,11 +6284,11 @@
       <c r="C32" s="151" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="175" t="s">
+      <c r="D32" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="176"/>
-      <c r="F32" s="176"/>
+      <c r="E32" s="224"/>
+      <c r="F32" s="224"/>
       <c r="G32" s="152"/>
       <c r="H32" s="155">
         <v>43774</v>
@@ -6308,11 +6308,11 @@
       <c r="C33" s="151" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="175" t="s">
+      <c r="D33" s="223" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="176"/>
-      <c r="F33" s="176"/>
+      <c r="E33" s="224"/>
+      <c r="F33" s="224"/>
       <c r="G33" s="152"/>
       <c r="H33" s="155">
         <v>43774</v>
@@ -6332,11 +6332,11 @@
       <c r="C34" s="151" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="175" t="s">
+      <c r="D34" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="176"/>
-      <c r="F34" s="176"/>
+      <c r="E34" s="224"/>
+      <c r="F34" s="224"/>
       <c r="G34" s="152"/>
       <c r="H34" s="155">
         <v>43774</v>
@@ -6356,11 +6356,11 @@
       <c r="C35" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="D35" s="175" t="s">
+      <c r="D35" s="223" t="s">
         <v>138</v>
       </c>
-      <c r="E35" s="176"/>
-      <c r="F35" s="176"/>
+      <c r="E35" s="224"/>
+      <c r="F35" s="224"/>
       <c r="G35" s="152"/>
       <c r="H35" s="155">
         <v>43774</v>
@@ -6380,11 +6380,11 @@
       <c r="C36" s="151" t="s">
         <v>139</v>
       </c>
-      <c r="D36" s="175" t="s">
+      <c r="D36" s="223" t="s">
         <v>138</v>
       </c>
-      <c r="E36" s="176"/>
-      <c r="F36" s="176"/>
+      <c r="E36" s="224"/>
+      <c r="F36" s="224"/>
       <c r="G36" s="152"/>
       <c r="H36" s="155">
         <v>43774</v>
@@ -6404,11 +6404,11 @@
       <c r="C37" s="151" t="s">
         <v>141</v>
       </c>
-      <c r="D37" s="175" t="s">
+      <c r="D37" s="223" t="s">
         <v>140</v>
       </c>
-      <c r="E37" s="176"/>
-      <c r="F37" s="176"/>
+      <c r="E37" s="224"/>
+      <c r="F37" s="224"/>
       <c r="G37" s="152"/>
       <c r="H37" s="155">
         <v>43774</v>
@@ -6428,11 +6428,11 @@
       <c r="C38" s="151" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="175" t="s">
+      <c r="D38" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
+      <c r="E38" s="224"/>
+      <c r="F38" s="224"/>
       <c r="G38" s="152"/>
       <c r="H38" s="155">
         <v>43774</v>
@@ -6452,11 +6452,11 @@
       <c r="C39" s="151" t="s">
         <v>144</v>
       </c>
-      <c r="D39" s="175" t="s">
+      <c r="D39" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E39" s="176"/>
-      <c r="F39" s="176"/>
+      <c r="E39" s="224"/>
+      <c r="F39" s="224"/>
       <c r="G39" s="152"/>
       <c r="H39" s="155">
         <v>43774</v>
@@ -6476,11 +6476,11 @@
       <c r="C40" s="151" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="175" t="s">
+      <c r="D40" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E40" s="176"/>
-      <c r="F40" s="176"/>
+      <c r="E40" s="224"/>
+      <c r="F40" s="224"/>
       <c r="G40" s="152"/>
       <c r="H40" s="155">
         <v>43774</v>
@@ -6500,11 +6500,11 @@
       <c r="C41" s="151" t="s">
         <v>147</v>
       </c>
-      <c r="D41" s="175" t="s">
+      <c r="D41" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="176"/>
-      <c r="F41" s="176"/>
+      <c r="E41" s="224"/>
+      <c r="F41" s="224"/>
       <c r="G41" s="152"/>
       <c r="H41" s="155">
         <v>43774</v>
@@ -6524,11 +6524,11 @@
       <c r="C42" s="151" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="175" t="s">
+      <c r="D42" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="176"/>
-      <c r="F42" s="176"/>
+      <c r="E42" s="224"/>
+      <c r="F42" s="224"/>
       <c r="G42" s="152"/>
       <c r="H42" s="155">
         <v>43774</v>
@@ -6548,11 +6548,11 @@
       <c r="C43" s="151" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="175" t="s">
+      <c r="D43" s="223" t="s">
         <v>153</v>
       </c>
-      <c r="E43" s="176"/>
-      <c r="F43" s="176"/>
+      <c r="E43" s="224"/>
+      <c r="F43" s="224"/>
       <c r="G43" s="152"/>
       <c r="H43" s="155">
         <v>43774</v>
@@ -6572,11 +6572,11 @@
       <c r="C44" s="151" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="175" t="s">
+      <c r="D44" s="223" t="s">
         <v>153</v>
       </c>
-      <c r="E44" s="176"/>
-      <c r="F44" s="176"/>
+      <c r="E44" s="224"/>
+      <c r="F44" s="224"/>
       <c r="G44" s="152"/>
       <c r="H44" s="155">
         <v>43774</v>
@@ -6596,11 +6596,11 @@
       <c r="C45" s="151" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="175" t="s">
+      <c r="D45" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E45" s="176"/>
-      <c r="F45" s="176"/>
+      <c r="E45" s="224"/>
+      <c r="F45" s="224"/>
       <c r="G45" s="152"/>
       <c r="H45" s="155">
         <v>43774</v>
@@ -6620,11 +6620,11 @@
       <c r="C46" s="151" t="s">
         <v>159</v>
       </c>
-      <c r="D46" s="175" t="s">
+      <c r="D46" s="223" t="s">
         <v>153</v>
       </c>
-      <c r="E46" s="176"/>
-      <c r="F46" s="176"/>
+      <c r="E46" s="224"/>
+      <c r="F46" s="224"/>
       <c r="G46" s="152"/>
       <c r="H46" s="155">
         <v>43774</v>
@@ -6644,11 +6644,11 @@
       <c r="C47" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="D47" s="175" t="s">
+      <c r="D47" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="176"/>
-      <c r="F47" s="176"/>
+      <c r="E47" s="224"/>
+      <c r="F47" s="224"/>
       <c r="G47" s="152"/>
       <c r="H47" s="155">
         <v>43774</v>
@@ -6668,11 +6668,11 @@
       <c r="C48" s="151" t="s">
         <v>163</v>
       </c>
-      <c r="D48" s="175" t="s">
+      <c r="D48" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E48" s="176"/>
-      <c r="F48" s="176"/>
+      <c r="E48" s="224"/>
+      <c r="F48" s="224"/>
       <c r="G48" s="152"/>
       <c r="H48" s="155">
         <v>43774</v>
@@ -6692,11 +6692,11 @@
       <c r="C49" s="151" t="s">
         <v>165</v>
       </c>
-      <c r="D49" s="175" t="s">
+      <c r="D49" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="176"/>
-      <c r="F49" s="176"/>
+      <c r="E49" s="224"/>
+      <c r="F49" s="224"/>
       <c r="G49" s="152"/>
       <c r="H49" s="155">
         <v>43774</v>
@@ -6716,11 +6716,11 @@
       <c r="C50" s="151" t="s">
         <v>167</v>
       </c>
-      <c r="D50" s="175" t="s">
+      <c r="D50" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E50" s="176"/>
-      <c r="F50" s="176"/>
+      <c r="E50" s="224"/>
+      <c r="F50" s="224"/>
       <c r="G50" s="152"/>
       <c r="H50" s="155">
         <v>43774</v>
@@ -6740,11 +6740,11 @@
       <c r="C51" s="151" t="s">
         <v>169</v>
       </c>
-      <c r="D51" s="175" t="s">
+      <c r="D51" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E51" s="176"/>
-      <c r="F51" s="176"/>
+      <c r="E51" s="224"/>
+      <c r="F51" s="224"/>
       <c r="G51" s="152"/>
       <c r="H51" s="155">
         <v>43774</v>
@@ -6764,11 +6764,11 @@
       <c r="C52" s="151" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="175" t="s">
+      <c r="D52" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E52" s="176"/>
-      <c r="F52" s="176"/>
+      <c r="E52" s="224"/>
+      <c r="F52" s="224"/>
       <c r="G52" s="152"/>
       <c r="H52" s="155">
         <v>43774</v>
@@ -6788,11 +6788,11 @@
       <c r="C53" s="151" t="s">
         <v>173</v>
       </c>
-      <c r="D53" s="175" t="s">
+      <c r="D53" s="223" t="s">
         <v>174</v>
       </c>
-      <c r="E53" s="176"/>
-      <c r="F53" s="176"/>
+      <c r="E53" s="224"/>
+      <c r="F53" s="224"/>
       <c r="G53" s="152"/>
       <c r="H53" s="155">
         <v>43774</v>
@@ -6812,11 +6812,11 @@
       <c r="C54" s="151" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="175" t="s">
+      <c r="D54" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="176"/>
-      <c r="F54" s="176"/>
+      <c r="E54" s="224"/>
+      <c r="F54" s="224"/>
       <c r="G54" s="152"/>
       <c r="H54" s="155">
         <v>43774</v>
@@ -6836,11 +6836,11 @@
       <c r="C55" s="151" t="s">
         <v>178</v>
       </c>
-      <c r="D55" s="175" t="s">
+      <c r="D55" s="223" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="176"/>
-      <c r="F55" s="176"/>
+      <c r="E55" s="224"/>
+      <c r="F55" s="224"/>
       <c r="G55" s="152"/>
       <c r="H55" s="155">
         <v>43774</v>
@@ -6860,11 +6860,11 @@
       <c r="C56" s="151" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="175" t="s">
+      <c r="D56" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E56" s="176"/>
-      <c r="F56" s="176"/>
+      <c r="E56" s="224"/>
+      <c r="F56" s="224"/>
       <c r="G56" s="152"/>
       <c r="H56" s="155">
         <v>43774</v>
@@ -6884,11 +6884,11 @@
       <c r="C57" s="151" t="s">
         <v>189</v>
       </c>
-      <c r="D57" s="175" t="s">
+      <c r="D57" s="223" t="s">
         <v>127</v>
       </c>
-      <c r="E57" s="176"/>
-      <c r="F57" s="176"/>
+      <c r="E57" s="224"/>
+      <c r="F57" s="224"/>
       <c r="G57" s="152"/>
       <c r="H57" s="155">
         <v>43774</v>
@@ -6908,11 +6908,11 @@
       <c r="C58" s="151" t="s">
         <v>190</v>
       </c>
-      <c r="D58" s="175" t="s">
+      <c r="D58" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E58" s="176"/>
-      <c r="F58" s="176"/>
+      <c r="E58" s="224"/>
+      <c r="F58" s="224"/>
       <c r="G58" s="152"/>
       <c r="H58" s="155">
         <v>43774</v>
@@ -6932,11 +6932,11 @@
       <c r="C59" s="151" t="s">
         <v>191</v>
       </c>
-      <c r="D59" s="175" t="s">
+      <c r="D59" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E59" s="176"/>
-      <c r="F59" s="176"/>
+      <c r="E59" s="224"/>
+      <c r="F59" s="224"/>
       <c r="G59" s="152"/>
       <c r="H59" s="155">
         <v>43774</v>
@@ -6956,11 +6956,11 @@
       <c r="C60" s="117" t="s">
         <v>192</v>
       </c>
-      <c r="D60" s="172" t="s">
+      <c r="D60" s="228" t="s">
         <v>128</v>
       </c>
-      <c r="E60" s="173"/>
-      <c r="F60" s="173"/>
+      <c r="E60" s="229"/>
+      <c r="F60" s="229"/>
       <c r="G60" s="118"/>
       <c r="H60" s="121">
         <v>43774</v>
@@ -6982,11 +6982,11 @@
       <c r="C61" s="151" t="s">
         <v>194</v>
       </c>
-      <c r="D61" s="175" t="s">
+      <c r="D61" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E61" s="176"/>
-      <c r="F61" s="176"/>
+      <c r="E61" s="224"/>
+      <c r="F61" s="224"/>
       <c r="G61" s="152"/>
       <c r="H61" s="155">
         <v>43774</v>
@@ -7006,11 +7006,11 @@
       <c r="C62" s="151" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="175" t="s">
+      <c r="D62" s="223" t="s">
         <v>128</v>
       </c>
-      <c r="E62" s="176"/>
-      <c r="F62" s="176"/>
+      <c r="E62" s="224"/>
+      <c r="F62" s="224"/>
       <c r="G62" s="152"/>
       <c r="H62" s="155">
         <v>43774</v>
@@ -7030,11 +7030,11 @@
       <c r="C63" s="151" t="s">
         <v>196</v>
       </c>
-      <c r="D63" s="175" t="s">
+      <c r="D63" s="223" t="s">
         <v>197</v>
       </c>
-      <c r="E63" s="176"/>
-      <c r="F63" s="176"/>
+      <c r="E63" s="224"/>
+      <c r="F63" s="224"/>
       <c r="G63" s="152"/>
       <c r="H63" s="155">
         <v>43774</v>
@@ -7054,11 +7054,11 @@
       <c r="C64" s="117" t="s">
         <v>199</v>
       </c>
-      <c r="D64" s="172" t="s">
+      <c r="D64" s="228" t="s">
         <v>127</v>
       </c>
-      <c r="E64" s="173"/>
-      <c r="F64" s="173"/>
+      <c r="E64" s="229"/>
+      <c r="F64" s="229"/>
       <c r="G64" s="118"/>
       <c r="H64" s="157">
         <v>43774</v>
@@ -7080,11 +7080,11 @@
       <c r="C65" s="151" t="s">
         <v>203</v>
       </c>
-      <c r="D65" s="181" t="s">
+      <c r="D65" s="230" t="s">
         <v>127</v>
       </c>
-      <c r="E65" s="182"/>
-      <c r="F65" s="182"/>
+      <c r="E65" s="231"/>
+      <c r="F65" s="231"/>
       <c r="G65" s="164"/>
       <c r="H65" s="155">
         <v>43774</v>
@@ -7104,11 +7104,11 @@
       <c r="C66" s="151" t="s">
         <v>205</v>
       </c>
-      <c r="D66" s="181" t="s">
+      <c r="D66" s="230" t="s">
         <v>128</v>
       </c>
-      <c r="E66" s="182"/>
-      <c r="F66" s="182"/>
+      <c r="E66" s="231"/>
+      <c r="F66" s="231"/>
       <c r="G66" s="164"/>
       <c r="H66" s="155">
         <v>43774</v>
@@ -7128,11 +7128,11 @@
       <c r="C67" s="151" t="s">
         <v>207</v>
       </c>
-      <c r="D67" s="181" t="s">
+      <c r="D67" s="230" t="s">
         <v>128</v>
       </c>
-      <c r="E67" s="182"/>
-      <c r="F67" s="182"/>
+      <c r="E67" s="231"/>
+      <c r="F67" s="231"/>
       <c r="G67" s="164"/>
       <c r="H67" s="155">
         <v>43774</v>
@@ -7152,11 +7152,11 @@
       <c r="C68" s="151" t="s">
         <v>209</v>
       </c>
-      <c r="D68" s="181" t="s">
+      <c r="D68" s="230" t="s">
         <v>128</v>
       </c>
-      <c r="E68" s="182"/>
-      <c r="F68" s="182"/>
+      <c r="E68" s="231"/>
+      <c r="F68" s="231"/>
       <c r="G68" s="164"/>
       <c r="H68" s="155">
         <v>43774</v>
@@ -7176,11 +7176,11 @@
       <c r="C69" s="117" t="s">
         <v>211</v>
       </c>
-      <c r="D69" s="183" t="s">
+      <c r="D69" s="234" t="s">
         <v>128</v>
       </c>
-      <c r="E69" s="184"/>
-      <c r="F69" s="184"/>
+      <c r="E69" s="235"/>
+      <c r="F69" s="235"/>
       <c r="G69" s="159"/>
       <c r="H69" s="121">
         <v>43774</v>
@@ -7202,11 +7202,11 @@
       <c r="C70" s="151" t="s">
         <v>98</v>
       </c>
-      <c r="D70" s="175" t="s">
+      <c r="D70" s="223" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="176"/>
-      <c r="F70" s="176"/>
+      <c r="E70" s="224"/>
+      <c r="F70" s="224"/>
       <c r="G70" s="152"/>
       <c r="H70" s="155">
         <v>43774</v>
@@ -7226,11 +7226,11 @@
       <c r="C71" s="151" t="s">
         <v>108</v>
       </c>
-      <c r="D71" s="175" t="s">
+      <c r="D71" s="223" t="s">
         <v>107</v>
       </c>
-      <c r="E71" s="176"/>
-      <c r="F71" s="176"/>
+      <c r="E71" s="224"/>
+      <c r="F71" s="224"/>
       <c r="G71" s="152"/>
       <c r="H71" s="155">
         <v>43774</v>
@@ -7250,11 +7250,11 @@
       <c r="C72" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="D72" s="178" t="s">
+      <c r="D72" s="183" t="s">
         <v>101</v>
       </c>
-      <c r="E72" s="179"/>
-      <c r="F72" s="179"/>
+      <c r="E72" s="184"/>
+      <c r="F72" s="184"/>
       <c r="G72" s="86"/>
       <c r="H72" s="123">
         <v>43774</v>
@@ -7274,11 +7274,11 @@
       <c r="C73" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="D73" s="178" t="s">
+      <c r="D73" s="183" t="s">
         <v>117</v>
       </c>
-      <c r="E73" s="179"/>
-      <c r="F73" s="179"/>
+      <c r="E73" s="184"/>
+      <c r="F73" s="184"/>
       <c r="G73" s="86"/>
       <c r="H73" s="122">
         <v>43774</v>
@@ -7298,11 +7298,11 @@
       <c r="C74" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="D74" s="178" t="s">
+      <c r="D74" s="183" t="s">
         <v>103</v>
       </c>
-      <c r="E74" s="179"/>
-      <c r="F74" s="179"/>
+      <c r="E74" s="184"/>
+      <c r="F74" s="184"/>
       <c r="G74" s="86"/>
       <c r="H74" s="122">
         <v>43774</v>
@@ -7322,11 +7322,11 @@
       <c r="C75" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="D75" s="178" t="s">
+      <c r="D75" s="183" t="s">
         <v>103</v>
       </c>
-      <c r="E75" s="179"/>
-      <c r="F75" s="180"/>
+      <c r="E75" s="184"/>
+      <c r="F75" s="214"/>
       <c r="G75" s="87"/>
       <c r="H75" s="122">
         <v>43774</v>
@@ -7346,11 +7346,11 @@
       <c r="C76" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="D76" s="178" t="s">
+      <c r="D76" s="183" t="s">
         <v>103</v>
       </c>
-      <c r="E76" s="179"/>
-      <c r="F76" s="180"/>
+      <c r="E76" s="184"/>
+      <c r="F76" s="214"/>
       <c r="G76" s="124"/>
       <c r="H76" s="122">
         <v>43774</v>
@@ -7370,11 +7370,11 @@
       <c r="C77" s="103" t="s">
         <v>222</v>
       </c>
-      <c r="D77" s="178" t="s">
+      <c r="D77" s="183" t="s">
         <v>101</v>
       </c>
-      <c r="E77" s="179"/>
-      <c r="F77" s="180"/>
+      <c r="E77" s="184"/>
+      <c r="F77" s="214"/>
       <c r="G77" s="124"/>
       <c r="H77" s="122">
         <v>43774</v>
@@ -7394,11 +7394,11 @@
       <c r="C78" s="103" t="s">
         <v>223</v>
       </c>
-      <c r="D78" s="178" t="s">
+      <c r="D78" s="183" t="s">
         <v>151</v>
       </c>
-      <c r="E78" s="179"/>
-      <c r="F78" s="180"/>
+      <c r="E78" s="184"/>
+      <c r="F78" s="214"/>
       <c r="G78" s="124"/>
       <c r="H78" s="122">
         <v>43774</v>
@@ -7418,11 +7418,11 @@
       <c r="C79" s="103" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="178" t="s">
+      <c r="D79" s="183" t="s">
         <v>226</v>
       </c>
-      <c r="E79" s="179"/>
-      <c r="F79" s="180"/>
+      <c r="E79" s="184"/>
+      <c r="F79" s="214"/>
       <c r="G79" s="124"/>
       <c r="H79" s="122">
         <v>43774</v>
@@ -7442,11 +7442,11 @@
       <c r="C80" s="103" t="s">
         <v>228</v>
       </c>
-      <c r="D80" s="178" t="s">
+      <c r="D80" s="183" t="s">
         <v>231</v>
       </c>
-      <c r="E80" s="179"/>
-      <c r="F80" s="180"/>
+      <c r="E80" s="184"/>
+      <c r="F80" s="214"/>
       <c r="G80" s="87"/>
       <c r="H80" s="122">
         <v>43774</v>
@@ -7466,11 +7466,11 @@
       <c r="C81" s="103" t="s">
         <v>230</v>
       </c>
-      <c r="D81" s="178" t="s">
+      <c r="D81" s="183" t="s">
         <v>232</v>
       </c>
-      <c r="E81" s="179"/>
-      <c r="F81" s="180"/>
+      <c r="E81" s="184"/>
+      <c r="F81" s="214"/>
       <c r="G81" s="124"/>
       <c r="H81" s="123">
         <v>43774</v>
@@ -7490,11 +7490,11 @@
       <c r="C82" s="103" t="s">
         <v>234</v>
       </c>
-      <c r="D82" s="178" t="s">
+      <c r="D82" s="183" t="s">
         <v>232</v>
       </c>
-      <c r="E82" s="179"/>
-      <c r="F82" s="180"/>
+      <c r="E82" s="184"/>
+      <c r="F82" s="214"/>
       <c r="G82" s="124"/>
       <c r="H82" s="123">
         <v>43774</v>
@@ -7514,11 +7514,11 @@
       <c r="C83" s="103" t="s">
         <v>238</v>
       </c>
-      <c r="D83" s="178" t="s">
+      <c r="D83" s="183" t="s">
         <v>232</v>
       </c>
-      <c r="E83" s="179"/>
-      <c r="F83" s="180"/>
+      <c r="E83" s="184"/>
+      <c r="F83" s="214"/>
       <c r="G83" s="124"/>
       <c r="H83" s="123">
         <v>43774</v>
@@ -7538,11 +7538,11 @@
       <c r="C84" s="103" t="s">
         <v>236</v>
       </c>
-      <c r="D84" s="178" t="s">
+      <c r="D84" s="183" t="s">
         <v>232</v>
       </c>
-      <c r="E84" s="179"/>
-      <c r="F84" s="180"/>
+      <c r="E84" s="184"/>
+      <c r="F84" s="214"/>
       <c r="G84" s="124"/>
       <c r="H84" s="123">
         <v>43774</v>
@@ -7562,11 +7562,11 @@
       <c r="C85" s="103" t="s">
         <v>240</v>
       </c>
-      <c r="D85" s="178" t="s">
+      <c r="D85" s="183" t="s">
         <v>241</v>
       </c>
-      <c r="E85" s="179"/>
-      <c r="F85" s="180"/>
+      <c r="E85" s="184"/>
+      <c r="F85" s="214"/>
       <c r="G85" s="124"/>
       <c r="H85" s="123">
         <v>43774</v>
@@ -7586,11 +7586,11 @@
       <c r="C86" s="124" t="s">
         <v>243</v>
       </c>
-      <c r="D86" s="178" t="s">
+      <c r="D86" s="183" t="s">
         <v>249</v>
       </c>
-      <c r="E86" s="179"/>
-      <c r="F86" s="180"/>
+      <c r="E86" s="184"/>
+      <c r="F86" s="214"/>
       <c r="G86" s="124"/>
       <c r="H86" s="123">
         <v>43774</v>
@@ -7612,11 +7612,11 @@
       <c r="C87" s="124" t="s">
         <v>246</v>
       </c>
-      <c r="D87" s="178" t="s">
+      <c r="D87" s="183" t="s">
         <v>248</v>
       </c>
-      <c r="E87" s="179"/>
-      <c r="F87" s="180"/>
+      <c r="E87" s="184"/>
+      <c r="F87" s="214"/>
       <c r="G87" s="124"/>
       <c r="H87" s="123">
         <v>43774</v>
@@ -7636,11 +7636,11 @@
       <c r="C88" s="124" t="s">
         <v>247</v>
       </c>
-      <c r="D88" s="178" t="s">
+      <c r="D88" s="183" t="s">
         <v>248</v>
       </c>
-      <c r="E88" s="179"/>
-      <c r="F88" s="180"/>
+      <c r="E88" s="184"/>
+      <c r="F88" s="214"/>
       <c r="G88" s="124"/>
       <c r="H88" s="123">
         <v>43774</v>
@@ -7660,11 +7660,11 @@
       <c r="C89" s="124" t="s">
         <v>250</v>
       </c>
-      <c r="D89" s="178" t="s">
+      <c r="D89" s="183" t="s">
         <v>248</v>
       </c>
-      <c r="E89" s="179"/>
-      <c r="F89" s="180"/>
+      <c r="E89" s="184"/>
+      <c r="F89" s="214"/>
       <c r="G89" s="124"/>
       <c r="H89" s="123">
         <v>43774</v>
@@ -7684,11 +7684,11 @@
       <c r="C90" s="124" t="s">
         <v>252</v>
       </c>
-      <c r="D90" s="178" t="s">
+      <c r="D90" s="183" t="s">
         <v>248</v>
       </c>
-      <c r="E90" s="179"/>
-      <c r="F90" s="180"/>
+      <c r="E90" s="184"/>
+      <c r="F90" s="214"/>
       <c r="G90" s="124"/>
       <c r="H90" s="123">
         <v>43774</v>
@@ -7708,11 +7708,11 @@
       <c r="C91" s="124" t="s">
         <v>254</v>
       </c>
-      <c r="D91" s="178" t="s">
+      <c r="D91" s="183" t="s">
         <v>248</v>
       </c>
-      <c r="E91" s="179"/>
-      <c r="F91" s="180"/>
+      <c r="E91" s="184"/>
+      <c r="F91" s="214"/>
       <c r="G91" s="124"/>
       <c r="H91" s="123">
         <v>43774</v>
@@ -7732,11 +7732,11 @@
       <c r="C92" s="124" t="s">
         <v>256</v>
       </c>
-      <c r="D92" s="178" t="s">
+      <c r="D92" s="183" t="s">
         <v>249</v>
       </c>
-      <c r="E92" s="179"/>
-      <c r="F92" s="180"/>
+      <c r="E92" s="184"/>
+      <c r="F92" s="214"/>
       <c r="G92" s="124"/>
       <c r="H92" s="123">
         <v>43774</v>
@@ -7756,11 +7756,11 @@
       <c r="C93" s="124" t="s">
         <v>258</v>
       </c>
-      <c r="D93" s="178" t="s">
+      <c r="D93" s="183" t="s">
         <v>249</v>
       </c>
-      <c r="E93" s="179"/>
-      <c r="F93" s="180"/>
+      <c r="E93" s="184"/>
+      <c r="F93" s="214"/>
       <c r="G93" s="124"/>
       <c r="H93" s="123">
         <v>43774</v>
@@ -7780,11 +7780,11 @@
       <c r="C94" s="119" t="s">
         <v>260</v>
       </c>
-      <c r="D94" s="172" t="s">
+      <c r="D94" s="228" t="s">
         <v>248</v>
       </c>
-      <c r="E94" s="173"/>
-      <c r="F94" s="174"/>
+      <c r="E94" s="229"/>
+      <c r="F94" s="232"/>
       <c r="G94" s="119"/>
       <c r="H94" s="168">
         <v>43774</v>
@@ -7806,11 +7806,11 @@
       <c r="C95" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="D95" s="175" t="s">
+      <c r="D95" s="223" t="s">
         <v>248</v>
       </c>
-      <c r="E95" s="176"/>
-      <c r="F95" s="177"/>
+      <c r="E95" s="224"/>
+      <c r="F95" s="233"/>
       <c r="G95" s="112"/>
       <c r="H95" s="169">
         <v>43774</v>
@@ -7830,11 +7830,11 @@
       <c r="C96" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D96" s="175" t="s">
+      <c r="D96" s="223" t="s">
         <v>248</v>
       </c>
-      <c r="E96" s="176"/>
-      <c r="F96" s="177"/>
+      <c r="E96" s="224"/>
+      <c r="F96" s="233"/>
       <c r="G96" s="112"/>
       <c r="H96" s="169">
         <v>43774</v>
@@ -7845,26 +7845,26 @@
       <c r="J96" s="153"/>
     </row>
     <row r="97" spans="1:14" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A97" s="185" t="s">
+      <c r="A97" s="211" t="s">
         <v>104</v>
       </c>
-      <c r="B97" s="186"/>
-      <c r="C97" s="186"/>
-      <c r="D97" s="186"/>
-      <c r="E97" s="186"/>
-      <c r="F97" s="186"/>
-      <c r="G97" s="186"/>
-      <c r="H97" s="186"/>
-      <c r="I97" s="186"/>
-      <c r="J97" s="187"/>
+      <c r="B97" s="212"/>
+      <c r="C97" s="212"/>
+      <c r="D97" s="212"/>
+      <c r="E97" s="212"/>
+      <c r="F97" s="212"/>
+      <c r="G97" s="212"/>
+      <c r="H97" s="212"/>
+      <c r="I97" s="212"/>
+      <c r="J97" s="213"/>
     </row>
     <row r="98" spans="1:14" s="4" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A98" s="88"/>
       <c r="B98" s="102"/>
       <c r="C98" s="103"/>
-      <c r="D98" s="196"/>
-      <c r="E98" s="179"/>
-      <c r="F98" s="179"/>
+      <c r="D98" s="215"/>
+      <c r="E98" s="184"/>
+      <c r="F98" s="184"/>
       <c r="G98" s="86"/>
       <c r="H98" s="135"/>
       <c r="I98" s="87"/>
@@ -7874,9 +7874,9 @@
       <c r="A99" s="88"/>
       <c r="B99" s="102"/>
       <c r="C99" s="103"/>
-      <c r="D99" s="196"/>
-      <c r="E99" s="179"/>
-      <c r="F99" s="179"/>
+      <c r="D99" s="215"/>
+      <c r="E99" s="184"/>
+      <c r="F99" s="184"/>
       <c r="G99" s="86"/>
       <c r="H99" s="135"/>
       <c r="I99" s="87"/>
@@ -7886,9 +7886,9 @@
       <c r="A100" s="88"/>
       <c r="B100" s="102"/>
       <c r="C100" s="103"/>
-      <c r="D100" s="196"/>
-      <c r="E100" s="179"/>
-      <c r="F100" s="179"/>
+      <c r="D100" s="215"/>
+      <c r="E100" s="184"/>
+      <c r="F100" s="184"/>
       <c r="G100" s="86"/>
       <c r="H100" s="136"/>
       <c r="I100" s="87"/>
@@ -7898,27 +7898,27 @@
       <c r="A101" s="88"/>
       <c r="B101" s="102"/>
       <c r="C101" s="103"/>
-      <c r="D101" s="196"/>
-      <c r="E101" s="179"/>
-      <c r="F101" s="179"/>
+      <c r="D101" s="215"/>
+      <c r="E101" s="184"/>
+      <c r="F101" s="184"/>
       <c r="G101" s="86"/>
       <c r="H101" s="135"/>
       <c r="I101" s="87"/>
       <c r="J101" s="85"/>
     </row>
     <row r="102" spans="1:14" s="4" customFormat="1" ht="12.75">
-      <c r="A102" s="185" t="s">
+      <c r="A102" s="211" t="s">
         <v>110</v>
       </c>
-      <c r="B102" s="186"/>
-      <c r="C102" s="186"/>
-      <c r="D102" s="186"/>
-      <c r="E102" s="186"/>
-      <c r="F102" s="186"/>
-      <c r="G102" s="186"/>
-      <c r="H102" s="186"/>
-      <c r="I102" s="186"/>
-      <c r="J102" s="187"/>
+      <c r="B102" s="212"/>
+      <c r="C102" s="212"/>
+      <c r="D102" s="212"/>
+      <c r="E102" s="212"/>
+      <c r="F102" s="212"/>
+      <c r="G102" s="212"/>
+      <c r="H102" s="212"/>
+      <c r="I102" s="212"/>
+      <c r="J102" s="213"/>
     </row>
     <row r="103" spans="1:14" s="93" customFormat="1" ht="62.25" customHeight="1" outlineLevel="1">
       <c r="A103" s="88" t="s">
@@ -7930,11 +7930,11 @@
       <c r="C103" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="D103" s="188" t="s">
+      <c r="D103" s="216" t="s">
         <v>112</v>
       </c>
-      <c r="E103" s="188"/>
-      <c r="F103" s="188"/>
+      <c r="E103" s="216"/>
+      <c r="F103" s="216"/>
       <c r="G103" s="130"/>
       <c r="H103" s="137">
         <v>43774</v>
@@ -7954,11 +7954,11 @@
       <c r="C104" s="126" t="s">
         <v>114</v>
       </c>
-      <c r="D104" s="191" t="s">
+      <c r="D104" s="221" t="s">
         <v>103</v>
       </c>
-      <c r="E104" s="192"/>
-      <c r="F104" s="192"/>
+      <c r="E104" s="222"/>
+      <c r="F104" s="222"/>
       <c r="G104" s="131"/>
       <c r="H104" s="141">
         <v>43774</v>
@@ -7968,33 +7968,33 @@
       </c>
       <c r="J104" s="128"/>
     </row>
-    <row r="105" spans="1:14" s="235" customFormat="1" ht="78" customHeight="1" outlineLevel="1">
+    <row r="105" spans="1:14" s="177" customFormat="1" ht="78" customHeight="1" outlineLevel="1">
       <c r="A105" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="B105" s="226" t="s">
+      <c r="B105" s="170" t="s">
         <v>113</v>
       </c>
-      <c r="C105" s="227" t="s">
+      <c r="C105" s="171" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="228" t="s">
+      <c r="D105" s="219" t="s">
         <v>119</v>
       </c>
-      <c r="E105" s="229"/>
-      <c r="F105" s="229"/>
-      <c r="G105" s="230"/>
-      <c r="H105" s="231">
+      <c r="E105" s="220"/>
+      <c r="F105" s="220"/>
+      <c r="G105" s="172"/>
+      <c r="H105" s="173">
         <v>43774</v>
       </c>
-      <c r="I105" s="232" t="s">
+      <c r="I105" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="J105" s="233"/>
-      <c r="K105" s="234"/>
-      <c r="L105" s="234"/>
-      <c r="M105" s="234"/>
-      <c r="N105" s="234"/>
+      <c r="J105" s="175"/>
+      <c r="K105" s="176"/>
+      <c r="L105" s="176"/>
+      <c r="M105" s="176"/>
+      <c r="N105" s="176"/>
     </row>
     <row r="106" spans="1:14" s="93" customFormat="1" ht="80.25" customHeight="1" outlineLevel="1">
       <c r="A106" s="143" t="s">
@@ -8006,11 +8006,11 @@
       <c r="C106" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="D106" s="189" t="s">
+      <c r="D106" s="217" t="s">
         <v>121</v>
       </c>
-      <c r="E106" s="190"/>
-      <c r="F106" s="190"/>
+      <c r="E106" s="218"/>
+      <c r="F106" s="218"/>
       <c r="G106" s="131"/>
       <c r="H106" s="146">
         <v>43774</v>
@@ -8030,51 +8030,51 @@
       <c r="C107" s="145" t="s">
         <v>123</v>
       </c>
-      <c r="D107" s="178" t="s">
+      <c r="D107" s="183" t="s">
         <v>124</v>
       </c>
-      <c r="E107" s="179"/>
-      <c r="F107" s="180"/>
+      <c r="E107" s="184"/>
+      <c r="F107" s="214"/>
       <c r="G107" s="130"/>
       <c r="H107" s="137"/>
       <c r="I107" s="142"/>
       <c r="J107" s="94"/>
     </row>
     <row r="108" spans="1:14" s="4" customFormat="1" ht="12.75">
-      <c r="A108" s="193" t="s">
+      <c r="A108" s="180" t="s">
         <v>42</v>
       </c>
-      <c r="B108" s="194"/>
-      <c r="C108" s="194"/>
-      <c r="D108" s="194"/>
-      <c r="E108" s="194"/>
-      <c r="F108" s="194"/>
-      <c r="G108" s="194"/>
-      <c r="H108" s="194"/>
-      <c r="I108" s="194"/>
-      <c r="J108" s="195"/>
+      <c r="B108" s="181"/>
+      <c r="C108" s="181"/>
+      <c r="D108" s="181"/>
+      <c r="E108" s="181"/>
+      <c r="F108" s="181"/>
+      <c r="G108" s="181"/>
+      <c r="H108" s="181"/>
+      <c r="I108" s="181"/>
+      <c r="J108" s="182"/>
     </row>
     <row r="109" spans="1:14" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A109" s="193" t="s">
+      <c r="A109" s="180" t="s">
         <v>59</v>
       </c>
-      <c r="B109" s="194"/>
-      <c r="C109" s="194"/>
-      <c r="D109" s="194"/>
-      <c r="E109" s="194"/>
-      <c r="F109" s="194"/>
-      <c r="G109" s="194"/>
-      <c r="H109" s="194"/>
-      <c r="I109" s="194"/>
-      <c r="J109" s="195"/>
+      <c r="B109" s="181"/>
+      <c r="C109" s="181"/>
+      <c r="D109" s="181"/>
+      <c r="E109" s="181"/>
+      <c r="F109" s="181"/>
+      <c r="G109" s="181"/>
+      <c r="H109" s="181"/>
+      <c r="I109" s="181"/>
+      <c r="J109" s="182"/>
     </row>
     <row r="110" spans="1:14" s="93" customFormat="1" ht="70.5" customHeight="1" outlineLevel="1">
       <c r="A110" s="88"/>
       <c r="B110" s="97"/>
       <c r="C110" s="92"/>
-      <c r="D110" s="178"/>
-      <c r="E110" s="179"/>
-      <c r="F110" s="179"/>
+      <c r="D110" s="183"/>
+      <c r="E110" s="184"/>
+      <c r="F110" s="184"/>
       <c r="G110" s="131"/>
       <c r="H110" s="138"/>
       <c r="I110" s="100"/>
@@ -8084,9 +8084,9 @@
       <c r="A111" s="88"/>
       <c r="B111" s="97"/>
       <c r="C111" s="92"/>
-      <c r="D111" s="178"/>
-      <c r="E111" s="179"/>
-      <c r="F111" s="179"/>
+      <c r="D111" s="183"/>
+      <c r="E111" s="184"/>
+      <c r="F111" s="184"/>
       <c r="G111" s="131"/>
       <c r="H111" s="138"/>
       <c r="I111" s="100"/>
@@ -8096,9 +8096,9 @@
       <c r="A112" s="88"/>
       <c r="B112" s="97"/>
       <c r="C112" s="92"/>
-      <c r="D112" s="178"/>
-      <c r="E112" s="179"/>
-      <c r="F112" s="179"/>
+      <c r="D112" s="183"/>
+      <c r="E112" s="184"/>
+      <c r="F112" s="184"/>
       <c r="G112" s="131"/>
       <c r="H112" s="138"/>
       <c r="I112" s="100"/>
@@ -8108,9 +8108,9 @@
       <c r="A113" s="88"/>
       <c r="B113" s="97"/>
       <c r="C113" s="92"/>
-      <c r="D113" s="178"/>
-      <c r="E113" s="179"/>
-      <c r="F113" s="179"/>
+      <c r="D113" s="183"/>
+      <c r="E113" s="184"/>
+      <c r="F113" s="184"/>
       <c r="G113" s="131"/>
       <c r="H113" s="138"/>
       <c r="I113" s="100"/>
@@ -8120,9 +8120,9 @@
       <c r="A114" s="88"/>
       <c r="B114" s="97"/>
       <c r="C114" s="92"/>
-      <c r="D114" s="178"/>
-      <c r="E114" s="179"/>
-      <c r="F114" s="179"/>
+      <c r="D114" s="183"/>
+      <c r="E114" s="184"/>
+      <c r="F114" s="184"/>
       <c r="G114" s="131"/>
       <c r="H114" s="138"/>
       <c r="I114" s="100"/>
@@ -8132,9 +8132,9 @@
       <c r="A115" s="88"/>
       <c r="B115" s="97"/>
       <c r="C115" s="92"/>
-      <c r="D115" s="178"/>
-      <c r="E115" s="179"/>
-      <c r="F115" s="179"/>
+      <c r="D115" s="183"/>
+      <c r="E115" s="184"/>
+      <c r="F115" s="184"/>
       <c r="G115" s="131"/>
       <c r="H115" s="138"/>
       <c r="I115" s="100"/>
@@ -8144,61 +8144,61 @@
       <c r="A116" s="88"/>
       <c r="B116" s="97"/>
       <c r="C116" s="92"/>
-      <c r="D116" s="178"/>
-      <c r="E116" s="179"/>
-      <c r="F116" s="179"/>
+      <c r="D116" s="183"/>
+      <c r="E116" s="184"/>
+      <c r="F116" s="184"/>
       <c r="G116" s="131"/>
       <c r="H116" s="138"/>
       <c r="I116" s="100"/>
       <c r="J116" s="94"/>
     </row>
     <row r="117" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A117" s="193" t="s">
+      <c r="A117" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="B117" s="194"/>
-      <c r="C117" s="194"/>
-      <c r="D117" s="194"/>
-      <c r="E117" s="194"/>
-      <c r="F117" s="194"/>
-      <c r="G117" s="194"/>
-      <c r="H117" s="194"/>
-      <c r="I117" s="194"/>
-      <c r="J117" s="195"/>
+      <c r="B117" s="181"/>
+      <c r="C117" s="181"/>
+      <c r="D117" s="181"/>
+      <c r="E117" s="181"/>
+      <c r="F117" s="181"/>
+      <c r="G117" s="181"/>
+      <c r="H117" s="181"/>
+      <c r="I117" s="181"/>
+      <c r="J117" s="182"/>
     </row>
     <row r="118" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A118" s="88"/>
       <c r="B118" s="97"/>
       <c r="C118" s="92"/>
-      <c r="D118" s="178"/>
-      <c r="E118" s="179"/>
-      <c r="F118" s="179"/>
+      <c r="D118" s="183"/>
+      <c r="E118" s="184"/>
+      <c r="F118" s="184"/>
       <c r="G118" s="131"/>
       <c r="H118" s="138"/>
       <c r="I118" s="100"/>
       <c r="J118" s="94"/>
     </row>
     <row r="119" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A119" s="193" t="s">
+      <c r="A119" s="180" t="s">
         <v>52</v>
       </c>
-      <c r="B119" s="194"/>
-      <c r="C119" s="194"/>
-      <c r="D119" s="194"/>
-      <c r="E119" s="194"/>
-      <c r="F119" s="194"/>
-      <c r="G119" s="194"/>
-      <c r="H119" s="194"/>
-      <c r="I119" s="194"/>
-      <c r="J119" s="195"/>
+      <c r="B119" s="181"/>
+      <c r="C119" s="181"/>
+      <c r="D119" s="181"/>
+      <c r="E119" s="181"/>
+      <c r="F119" s="181"/>
+      <c r="G119" s="181"/>
+      <c r="H119" s="181"/>
+      <c r="I119" s="181"/>
+      <c r="J119" s="182"/>
     </row>
     <row r="120" spans="1:10" s="93" customFormat="1" ht="101.25" customHeight="1" outlineLevel="1">
       <c r="A120" s="88"/>
       <c r="B120" s="97"/>
       <c r="C120" s="92"/>
-      <c r="D120" s="178"/>
-      <c r="E120" s="179"/>
-      <c r="F120" s="179"/>
+      <c r="D120" s="183"/>
+      <c r="E120" s="184"/>
+      <c r="F120" s="184"/>
       <c r="G120" s="131"/>
       <c r="H120" s="138"/>
       <c r="I120" s="106"/>
@@ -8208,9 +8208,9 @@
       <c r="A121" s="88"/>
       <c r="B121" s="97"/>
       <c r="C121" s="92"/>
-      <c r="D121" s="178"/>
-      <c r="E121" s="179"/>
-      <c r="F121" s="179"/>
+      <c r="D121" s="183"/>
+      <c r="E121" s="184"/>
+      <c r="F121" s="184"/>
       <c r="G121" s="131"/>
       <c r="H121" s="138"/>
       <c r="I121" s="100"/>
@@ -8220,35 +8220,35 @@
       <c r="A122" s="88"/>
       <c r="B122" s="97"/>
       <c r="C122" s="92"/>
-      <c r="D122" s="178"/>
-      <c r="E122" s="179"/>
-      <c r="F122" s="179"/>
+      <c r="D122" s="183"/>
+      <c r="E122" s="184"/>
+      <c r="F122" s="184"/>
       <c r="G122" s="131"/>
       <c r="H122" s="138"/>
       <c r="I122" s="100"/>
       <c r="J122" s="94"/>
     </row>
     <row r="123" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A123" s="193" t="s">
+      <c r="A123" s="180" t="s">
         <v>53</v>
       </c>
-      <c r="B123" s="194"/>
-      <c r="C123" s="194"/>
-      <c r="D123" s="194"/>
-      <c r="E123" s="194"/>
-      <c r="F123" s="194"/>
-      <c r="G123" s="194"/>
-      <c r="H123" s="194"/>
-      <c r="I123" s="194"/>
-      <c r="J123" s="195"/>
+      <c r="B123" s="181"/>
+      <c r="C123" s="181"/>
+      <c r="D123" s="181"/>
+      <c r="E123" s="181"/>
+      <c r="F123" s="181"/>
+      <c r="G123" s="181"/>
+      <c r="H123" s="181"/>
+      <c r="I123" s="181"/>
+      <c r="J123" s="182"/>
     </row>
     <row r="124" spans="1:10" s="93" customFormat="1" ht="27.75" customHeight="1" outlineLevel="1">
       <c r="A124" s="88"/>
       <c r="B124" s="97"/>
       <c r="C124" s="92"/>
-      <c r="D124" s="178"/>
-      <c r="E124" s="179"/>
-      <c r="F124" s="179"/>
+      <c r="D124" s="183"/>
+      <c r="E124" s="184"/>
+      <c r="F124" s="184"/>
       <c r="G124" s="131"/>
       <c r="H124" s="138"/>
       <c r="I124" s="100"/>
@@ -8258,49 +8258,49 @@
       <c r="A125" s="88"/>
       <c r="B125" s="97"/>
       <c r="C125" s="92"/>
-      <c r="D125" s="225"/>
-      <c r="E125" s="179"/>
-      <c r="F125" s="179"/>
+      <c r="D125" s="185"/>
+      <c r="E125" s="184"/>
+      <c r="F125" s="184"/>
       <c r="G125" s="131"/>
       <c r="H125" s="138"/>
       <c r="I125" s="100"/>
       <c r="J125" s="94"/>
     </row>
     <row r="126" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A126" s="193" t="s">
+      <c r="A126" s="180" t="s">
         <v>54</v>
       </c>
-      <c r="B126" s="194"/>
-      <c r="C126" s="194"/>
-      <c r="D126" s="194"/>
-      <c r="E126" s="194"/>
-      <c r="F126" s="194"/>
-      <c r="G126" s="194"/>
-      <c r="H126" s="194"/>
-      <c r="I126" s="194"/>
-      <c r="J126" s="195"/>
+      <c r="B126" s="181"/>
+      <c r="C126" s="181"/>
+      <c r="D126" s="181"/>
+      <c r="E126" s="181"/>
+      <c r="F126" s="181"/>
+      <c r="G126" s="181"/>
+      <c r="H126" s="181"/>
+      <c r="I126" s="181"/>
+      <c r="J126" s="182"/>
     </row>
     <row r="127" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A127" s="193" t="s">
+      <c r="A127" s="180" t="s">
         <v>55</v>
       </c>
-      <c r="B127" s="194"/>
-      <c r="C127" s="194"/>
-      <c r="D127" s="194"/>
-      <c r="E127" s="194"/>
-      <c r="F127" s="194"/>
-      <c r="G127" s="194"/>
-      <c r="H127" s="194"/>
-      <c r="I127" s="194"/>
-      <c r="J127" s="195"/>
+      <c r="B127" s="181"/>
+      <c r="C127" s="181"/>
+      <c r="D127" s="181"/>
+      <c r="E127" s="181"/>
+      <c r="F127" s="181"/>
+      <c r="G127" s="181"/>
+      <c r="H127" s="181"/>
+      <c r="I127" s="181"/>
+      <c r="J127" s="182"/>
     </row>
     <row r="128" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A128" s="88"/>
       <c r="B128" s="97"/>
       <c r="C128" s="92"/>
-      <c r="D128" s="178"/>
-      <c r="E128" s="179"/>
-      <c r="F128" s="179"/>
+      <c r="D128" s="183"/>
+      <c r="E128" s="184"/>
+      <c r="F128" s="184"/>
       <c r="G128" s="131"/>
       <c r="H128" s="138"/>
       <c r="I128" s="100"/>
@@ -8310,35 +8310,35 @@
       <c r="A129" s="88"/>
       <c r="B129" s="97"/>
       <c r="C129" s="92"/>
-      <c r="D129" s="178"/>
-      <c r="E129" s="179"/>
-      <c r="F129" s="179"/>
+      <c r="D129" s="183"/>
+      <c r="E129" s="184"/>
+      <c r="F129" s="184"/>
       <c r="G129" s="131"/>
       <c r="H129" s="138"/>
       <c r="I129" s="100"/>
       <c r="J129" s="94"/>
     </row>
     <row r="130" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A130" s="193" t="s">
+      <c r="A130" s="180" t="s">
         <v>56</v>
       </c>
-      <c r="B130" s="194"/>
-      <c r="C130" s="194"/>
-      <c r="D130" s="194"/>
-      <c r="E130" s="194"/>
-      <c r="F130" s="194"/>
-      <c r="G130" s="194"/>
-      <c r="H130" s="194"/>
-      <c r="I130" s="194"/>
-      <c r="J130" s="195"/>
+      <c r="B130" s="181"/>
+      <c r="C130" s="181"/>
+      <c r="D130" s="181"/>
+      <c r="E130" s="181"/>
+      <c r="F130" s="181"/>
+      <c r="G130" s="181"/>
+      <c r="H130" s="181"/>
+      <c r="I130" s="181"/>
+      <c r="J130" s="182"/>
     </row>
     <row r="131" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A131" s="88"/>
       <c r="B131" s="97"/>
       <c r="C131" s="92"/>
-      <c r="D131" s="178"/>
-      <c r="E131" s="179"/>
-      <c r="F131" s="179"/>
+      <c r="D131" s="183"/>
+      <c r="E131" s="184"/>
+      <c r="F131" s="184"/>
       <c r="G131" s="131"/>
       <c r="H131" s="138"/>
       <c r="I131" s="100"/>
@@ -8348,35 +8348,35 @@
       <c r="A132" s="88"/>
       <c r="B132" s="97"/>
       <c r="C132" s="92"/>
-      <c r="D132" s="178"/>
-      <c r="E132" s="179"/>
-      <c r="F132" s="179"/>
+      <c r="D132" s="183"/>
+      <c r="E132" s="184"/>
+      <c r="F132" s="184"/>
       <c r="G132" s="131"/>
       <c r="H132" s="138"/>
       <c r="I132" s="100"/>
       <c r="J132" s="94"/>
     </row>
     <row r="133" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A133" s="193" t="s">
+      <c r="A133" s="180" t="s">
         <v>57</v>
       </c>
-      <c r="B133" s="194"/>
-      <c r="C133" s="194"/>
-      <c r="D133" s="194"/>
-      <c r="E133" s="194"/>
-      <c r="F133" s="194"/>
-      <c r="G133" s="194"/>
-      <c r="H133" s="194"/>
-      <c r="I133" s="194"/>
-      <c r="J133" s="195"/>
+      <c r="B133" s="181"/>
+      <c r="C133" s="181"/>
+      <c r="D133" s="181"/>
+      <c r="E133" s="181"/>
+      <c r="F133" s="181"/>
+      <c r="G133" s="181"/>
+      <c r="H133" s="181"/>
+      <c r="I133" s="181"/>
+      <c r="J133" s="182"/>
     </row>
     <row r="134" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A134" s="88"/>
       <c r="B134" s="97"/>
       <c r="C134" s="92"/>
-      <c r="D134" s="178"/>
-      <c r="E134" s="179"/>
-      <c r="F134" s="179"/>
+      <c r="D134" s="183"/>
+      <c r="E134" s="184"/>
+      <c r="F134" s="184"/>
       <c r="G134" s="131"/>
       <c r="H134" s="138"/>
       <c r="I134" s="100"/>
@@ -8386,35 +8386,35 @@
       <c r="A135" s="88"/>
       <c r="B135" s="97"/>
       <c r="C135" s="92"/>
-      <c r="D135" s="178"/>
-      <c r="E135" s="179"/>
-      <c r="F135" s="179"/>
+      <c r="D135" s="183"/>
+      <c r="E135" s="184"/>
+      <c r="F135" s="184"/>
       <c r="G135" s="131"/>
       <c r="H135" s="138"/>
       <c r="I135" s="100"/>
       <c r="J135" s="94"/>
     </row>
     <row r="136" spans="1:10" s="4" customFormat="1" ht="12.75" outlineLevel="1">
-      <c r="A136" s="193" t="s">
+      <c r="A136" s="180" t="s">
         <v>58</v>
       </c>
-      <c r="B136" s="194"/>
-      <c r="C136" s="194"/>
-      <c r="D136" s="194"/>
-      <c r="E136" s="194"/>
-      <c r="F136" s="194"/>
-      <c r="G136" s="194"/>
-      <c r="H136" s="194"/>
-      <c r="I136" s="194"/>
-      <c r="J136" s="195"/>
+      <c r="B136" s="181"/>
+      <c r="C136" s="181"/>
+      <c r="D136" s="181"/>
+      <c r="E136" s="181"/>
+      <c r="F136" s="181"/>
+      <c r="G136" s="181"/>
+      <c r="H136" s="181"/>
+      <c r="I136" s="181"/>
+      <c r="J136" s="182"/>
     </row>
     <row r="137" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A137" s="88"/>
       <c r="B137" s="97"/>
       <c r="C137" s="92"/>
-      <c r="D137" s="178"/>
-      <c r="E137" s="179"/>
-      <c r="F137" s="179"/>
+      <c r="D137" s="183"/>
+      <c r="E137" s="184"/>
+      <c r="F137" s="184"/>
       <c r="G137" s="131"/>
       <c r="H137" s="138"/>
       <c r="I137" s="100"/>
@@ -8424,35 +8424,35 @@
       <c r="A138" s="88"/>
       <c r="B138" s="97"/>
       <c r="C138" s="92"/>
-      <c r="D138" s="178"/>
-      <c r="E138" s="179"/>
-      <c r="F138" s="179"/>
+      <c r="D138" s="183"/>
+      <c r="E138" s="184"/>
+      <c r="F138" s="184"/>
       <c r="G138" s="131"/>
       <c r="H138" s="138"/>
       <c r="I138" s="100"/>
       <c r="J138" s="94"/>
     </row>
     <row r="139" spans="1:10" s="4" customFormat="1" ht="12.75">
-      <c r="A139" s="193" t="s">
+      <c r="A139" s="180" t="s">
         <v>61</v>
       </c>
-      <c r="B139" s="194"/>
-      <c r="C139" s="194"/>
-      <c r="D139" s="194"/>
-      <c r="E139" s="194"/>
-      <c r="F139" s="194"/>
-      <c r="G139" s="194"/>
-      <c r="H139" s="194"/>
-      <c r="I139" s="194"/>
-      <c r="J139" s="195"/>
+      <c r="B139" s="181"/>
+      <c r="C139" s="181"/>
+      <c r="D139" s="181"/>
+      <c r="E139" s="181"/>
+      <c r="F139" s="181"/>
+      <c r="G139" s="181"/>
+      <c r="H139" s="181"/>
+      <c r="I139" s="181"/>
+      <c r="J139" s="182"/>
     </row>
     <row r="140" spans="1:10" s="93" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A140" s="88"/>
       <c r="B140" s="97"/>
       <c r="C140" s="92"/>
-      <c r="D140" s="178"/>
-      <c r="E140" s="179"/>
-      <c r="F140" s="179"/>
+      <c r="D140" s="183"/>
+      <c r="E140" s="184"/>
+      <c r="F140" s="184"/>
       <c r="G140" s="131"/>
       <c r="H140" s="138"/>
       <c r="I140" s="100"/>
@@ -8462,9 +8462,9 @@
       <c r="A141" s="88"/>
       <c r="B141" s="97"/>
       <c r="C141" s="92"/>
-      <c r="D141" s="178"/>
-      <c r="E141" s="179"/>
-      <c r="F141" s="179"/>
+      <c r="D141" s="183"/>
+      <c r="E141" s="184"/>
+      <c r="F141" s="184"/>
       <c r="G141" s="131"/>
       <c r="H141" s="138"/>
       <c r="I141" s="100"/>
@@ -8510,105 +8510,15 @@
     <row r="179" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="A139:J139"/>
-    <mergeCell ref="D140:F140"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="D135:F135"/>
-    <mergeCell ref="A136:J136"/>
-    <mergeCell ref="D137:F137"/>
-    <mergeCell ref="D138:F138"/>
-    <mergeCell ref="D131:F131"/>
-    <mergeCell ref="D132:F132"/>
-    <mergeCell ref="D134:F134"/>
-    <mergeCell ref="D128:F128"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="A127:J127"/>
-    <mergeCell ref="A130:J130"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D115:F115"/>
-    <mergeCell ref="A123:J123"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="A133:J133"/>
-    <mergeCell ref="A126:J126"/>
-    <mergeCell ref="D124:F124"/>
-    <mergeCell ref="D125:F125"/>
-    <mergeCell ref="A117:J117"/>
-    <mergeCell ref="A119:J119"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:G10"/>
-    <mergeCell ref="A97:J97"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="A109:J109"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="D99:F99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="A102:J102"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="A108:J108"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D77:F77"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="A24:J24"/>
@@ -8633,6 +8543,18 @@
     <mergeCell ref="D50:F50"/>
     <mergeCell ref="D51:F51"/>
     <mergeCell ref="D74:F74"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D36:F36"/>
     <mergeCell ref="D72:F72"/>
     <mergeCell ref="D70:F70"/>
     <mergeCell ref="D61:F61"/>
@@ -8645,19 +8567,97 @@
     <mergeCell ref="D58:F58"/>
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="A108:J108"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="A109:J109"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="D99:F99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="A102:J102"/>
+    <mergeCell ref="D101:F101"/>
     <mergeCell ref="D94:F94"/>
     <mergeCell ref="D95:F95"/>
     <mergeCell ref="D96:F96"/>
     <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D115:F115"/>
+    <mergeCell ref="A123:J123"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="A133:J133"/>
+    <mergeCell ref="A126:J126"/>
+    <mergeCell ref="D124:F124"/>
+    <mergeCell ref="D125:F125"/>
+    <mergeCell ref="A117:J117"/>
+    <mergeCell ref="A119:J119"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="A139:J139"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D135:F135"/>
+    <mergeCell ref="A136:J136"/>
+    <mergeCell ref="D137:F137"/>
+    <mergeCell ref="D138:F138"/>
+    <mergeCell ref="D131:F131"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="A127:J127"/>
+    <mergeCell ref="A130:J130"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>